<commit_message>
Trim function is added
Trim function is added
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DivyaDevanathan\git\SeleniumAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC068F4-5B52-45CC-9948-AE5879A02832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A993478F-5111-4C7C-8CF0-A83BDB077D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -504,13 +504,13 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1"/>
     <col min="5" max="5" width="47.28515625" customWidth="1"/>

</xml_diff>

<commit_message>
Implemented the config for Set create
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DivyaDevanathan\git\SeleniumAutomation\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC068F4-5B52-45CC-9948-AE5879A02832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1029E0D-1F10-4774-B249-1DC9B95A225F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Skin Care, This is to analyse about the skin</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>VerifyLoginPage_Test</t>
+  </si>
+  <si>
+    <t>CreateSet_Test</t>
+  </si>
+  <si>
+    <t>Create_Set</t>
+  </si>
+  <si>
+    <t>Create Set1,Disease,kera</t>
   </si>
 </sst>
 </file>
@@ -191,8 +200,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}" name="Table2" displayName="Table2" ref="A1:E10" totalsRowShown="0">
-  <autoFilter ref="A1:E10" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}" name="Table2" displayName="Table2" ref="A1:E11" totalsRowShown="0">
+  <autoFilter ref="A1:E11" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{86135FFC-C988-4F48-82DC-A41C181BA09E}" name="Test Case#"/>
     <tableColumn id="5" xr3:uid="{C46EA655-3EFD-4B21-A644-8A7F51CB4F27}" name="FunctionName"/>
@@ -501,16 +510,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1"/>
     <col min="5" max="5" width="47.28515625" customWidth="1"/>
@@ -550,91 +559,102 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated investigation test as per demo comments
updated investigation test as per demo comments
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DivyaDevanathan\git\SeleniumAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E89541-B576-4DFD-AEF0-9E2498A9302D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C996635-3E45-4E08-BB69-909C32D10F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Test Case#</t>
   </si>
@@ -99,29 +99,59 @@
     <t>DeleteInvestigation_Test</t>
   </si>
   <si>
-    <t>&lt;SetName&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ExplortionName&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Comparison&gt;</t>
-  </si>
-  <si>
-    <t>divya.devanathan@eaglegenomics.com</t>
-  </si>
-  <si>
-    <t>createone,Corona, To analysis the impact of the virus</t>
-  </si>
-  <si>
     <t>Skin Care, This is to analyse about the skin</t>
+  </si>
+  <si>
+    <t>&lt;InvestigationName&gt;,&lt;InvestigationDescription&gt;</t>
+  </si>
+  <si>
+    <t>&lt;InvestigationNameOld&gt;,&lt;InvestigationNameNew&gt;&lt;InvestigationDescription&gt;</t>
+  </si>
+  <si>
+    <t>&lt;InvestigationName&gt;</t>
+  </si>
+  <si>
+    <t>&lt;InvestigationName&gt;,&lt;Comparison&gt;</t>
+  </si>
+  <si>
+    <t>&lt;InvestigationName&gt;,&lt;ExplortionName&gt;</t>
+  </si>
+  <si>
+    <t>&lt;InvestigationName&gt;,&lt;SetName&gt;</t>
+  </si>
+  <si>
+    <t>&lt;InvestigationName&gt;,&lt;tobeShared&gt;</t>
+  </si>
+  <si>
+    <t>&lt;InvestigationName&gt;,&lt;toBeDeleted&gt;</t>
+  </si>
+  <si>
+    <t>Investigation1,modified, To analysis the impact of the virus</t>
+  </si>
+  <si>
+    <t>InvSet,Set1</t>
+  </si>
+  <si>
+    <t>InvShare,divya.devanathan@eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>InvDelete</t>
+  </si>
+  <si>
+    <t>Gene_invet</t>
+  </si>
+  <si>
+    <t>InvExploration,Explo1</t>
+  </si>
+  <si>
+    <t>InvComparison,Comp1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +163,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -159,15 +197,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <i/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -180,10 +225,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}" name="Table2" displayName="Table2" ref="A1:E9" totalsRowShown="0">
   <autoFilter ref="A1:E9" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}"/>
@@ -191,7 +232,7 @@
     <tableColumn id="1" xr3:uid="{86135FFC-C988-4F48-82DC-A41C181BA09E}" name="Test Case#"/>
     <tableColumn id="5" xr3:uid="{C46EA655-3EFD-4B21-A644-8A7F51CB4F27}" name="FunctionName"/>
     <tableColumn id="2" xr3:uid="{FDAD99A8-3FCD-465F-B419-AAFB06B7EA4E}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{4730EDB2-8FEB-4FAE-97C5-547308A4D4D9}" name="Test Steps"/>
+    <tableColumn id="3" xr3:uid="{4730EDB2-8FEB-4FAE-97C5-547308A4D4D9}" name="Test Steps" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{F14B9AFB-5FBF-49C3-808B-BAEB38FB0B82}" name="Test Data"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -497,16 +538,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -520,7 +561,7 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
@@ -534,8 +575,11 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -545,6 +589,12 @@
       <c r="B3" t="s">
         <v>14</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -553,8 +603,11 @@
       <c r="B4" t="s">
         <v>15</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -564,8 +617,11 @@
       <c r="B5" t="s">
         <v>16</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -575,8 +631,11 @@
       <c r="B6" t="s">
         <v>17</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -586,8 +645,11 @@
       <c r="B7" t="s">
         <v>18</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -597,8 +659,11 @@
       <c r="B8" t="s">
         <v>19</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -608,10 +673,16 @@
       <c r="B9" t="s">
         <v>20</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1" xr:uid="{B05D78C8-8588-4A6E-B0B2-FD1B5AD85FBB}"/>
+    <hyperlink ref="E8" r:id="rId1" display="divya.devanathan@eaglegenomics.com" xr:uid="{B05D78C8-8588-4A6E-B0B2-FD1B5AD85FBB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
updated after fix for  full run  in VM
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F40269-68C7-4479-B2F0-816643CA01C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272DD84B-525E-42CC-92D8-739697C51601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -909,9 +909,6 @@
     <t>Comparison Control and Case 2, Control Set, Case Set,Disease, kera,buy</t>
   </si>
   <si>
-    <t>Comparison Control and Case 1, Disease, Case Set2,soy</t>
-  </si>
-  <si>
     <t>Search a value in Comparison  in expanded view</t>
   </si>
   <si>
@@ -1138,6 +1135,9 @@
   </si>
   <si>
     <t>ComAddfromFile 1,Control Card, Disease,kera,Disease, C:\Users\MugunthRaman\git\EagleAutomation\Resources\Q4 - Upload file - 1 (2).xlsx, Q4 - Upload file - 1 (2).xlsx</t>
+  </si>
+  <si>
+    <t>Comparison Control and Case 1_222840, Disease, Case Set2,sor</t>
   </si>
 </sst>
 </file>
@@ -1895,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="D50" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,7 +1929,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1955,35 +1955,35 @@
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>356</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>357</v>
       </c>
       <c r="E3" s="5"/>
       <c r="G3" s="35" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E4" s="7"/>
       <c r="G4" s="36"/>
@@ -1991,16 +1991,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E5" s="7"/>
       <c r="G5" s="36"/>
@@ -2008,16 +2008,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E6" s="7"/>
       <c r="G6" s="36"/>
@@ -2025,16 +2025,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E7" s="7"/>
       <c r="G7" s="36"/>
@@ -2042,16 +2042,16 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>343</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>344</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>351</v>
-      </c>
       <c r="D8" s="26" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E8" s="9"/>
       <c r="G8" s="36"/>
@@ -2111,7 +2111,7 @@
         <v>79</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G11" s="31"/>
       <c r="H11" s="14"/>
@@ -2184,7 +2184,7 @@
         <v>84</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>86</v>
@@ -2206,7 +2206,7 @@
         <v>100</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G16" s="31"/>
       <c r="H16" s="14"/>
@@ -2480,7 +2480,7 @@
         <v>164</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G30" s="33"/>
       <c r="H30" s="14"/>
@@ -2613,7 +2613,7 @@
         <v>176</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G37" s="33"/>
       <c r="H37" s="14"/>
@@ -2767,7 +2767,7 @@
         <v>188</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G45" s="33"/>
       <c r="H45" s="14"/>
@@ -2786,7 +2786,7 @@
         <v>189</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G46" s="33"/>
       <c r="H46" s="17" t="s">
@@ -2868,7 +2868,7 @@
         <v>272</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G50" s="33"/>
       <c r="H50" s="14"/>
@@ -2884,7 +2884,7 @@
         <v>286</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>289</v>
@@ -2903,7 +2903,7 @@
         <v>287</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>290</v>
@@ -2922,10 +2922,10 @@
         <v>288</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>291</v>
+        <v>367</v>
       </c>
       <c r="G53" s="33"/>
       <c r="H53" s="14"/>
@@ -2938,13 +2938,13 @@
         <v>230</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G54" s="33"/>
       <c r="H54" s="14"/>
@@ -2957,13 +2957,13 @@
         <v>231</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G55" s="33"/>
       <c r="H55" s="14"/>
@@ -2976,13 +2976,13 @@
         <v>232</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D56" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="E56" s="7" t="s">
         <v>304</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>305</v>
       </c>
       <c r="G56" s="33"/>
       <c r="H56" s="14"/>
@@ -2995,13 +2995,13 @@
         <v>233</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G57" s="33"/>
       <c r="H57" s="14"/>
@@ -3014,13 +3014,13 @@
         <v>234</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G58" s="33"/>
       <c r="H58" s="14"/>
@@ -3033,13 +3033,13 @@
         <v>235</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G59" s="33"/>
       <c r="H59" s="14"/>
@@ -3052,13 +3052,13 @@
         <v>236</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>100</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G60" s="33"/>
       <c r="H60" s="14"/>
@@ -3071,13 +3071,13 @@
         <v>237</v>
       </c>
       <c r="C61" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="D61" s="6" t="s">
-        <v>317</v>
-      </c>
       <c r="E61" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G61" s="33"/>
       <c r="H61" s="14"/>
@@ -3090,13 +3090,13 @@
         <v>238</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G62" s="33"/>
       <c r="H62" s="14"/>
@@ -3112,10 +3112,10 @@
         <v>273</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G63" s="33"/>
       <c r="H63" s="14"/>
@@ -3131,10 +3131,10 @@
         <v>274</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G64" s="33"/>
       <c r="H64" s="14"/>
@@ -3150,10 +3150,10 @@
         <v>275</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G65" s="33"/>
       <c r="H65" s="14"/>
@@ -3169,10 +3169,10 @@
         <v>276</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G66" s="33"/>
       <c r="H66" s="14"/>
@@ -3188,10 +3188,10 @@
         <v>277</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G67" s="33"/>
       <c r="H67" s="14"/>
@@ -3204,13 +3204,13 @@
         <v>244</v>
       </c>
       <c r="C68" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D68" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="E68" s="7" t="s">
         <v>332</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>333</v>
       </c>
       <c r="G68" s="33"/>
       <c r="H68" s="14"/>
@@ -3226,10 +3226,10 @@
         <v>278</v>
       </c>
       <c r="D69" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E69" s="7" t="s">
         <v>335</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>336</v>
       </c>
       <c r="G69" s="33"/>
       <c r="H69" s="14"/>
@@ -3248,7 +3248,7 @@
         <v>189</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G70" s="33"/>
       <c r="H70" s="14"/>
@@ -3267,7 +3267,7 @@
         <v>190</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G71" s="33"/>
       <c r="H71" s="14"/>
@@ -3396,20 +3396,20 @@
     </row>
     <row r="80" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="27" t="s">
+        <v>359</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>361</v>
-      </c>
       <c r="D80" s="28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E80" s="3"/>
       <c r="G80" s="29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H80" s="14"/>
     </row>

</xml_diff>

<commit_message>
All the additional wait times are removed and minor change in configuration files
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272DD84B-525E-42CC-92D8-739697C51601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2112F9-9A64-475F-B894-E4065A2BB875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -954,9 +954,6 @@
     <t>SetAdd 1, Disease, aber,ComAddFromSet, Control Card,dol</t>
   </si>
   <si>
-    <t>DComparison2Card, Control Card,Case Card ,Disease, kera,lor</t>
-  </si>
-  <si>
     <t>&lt;Comparison Name to be selected&gt;,&lt;Control Set Name&gt;,&lt;Case Set Name&gt;,&lt;entity to be selected&gt;,&lt;search text for creating Comparison control&gt;, &lt;search text for creating Comparison case&gt;</t>
   </si>
   <si>
@@ -1138,6 +1135,9 @@
   </si>
   <si>
     <t>Comparison Control and Case 1_222840, Disease, Case Set2,sor</t>
+  </si>
+  <si>
+    <t>DComparison2Card, Control Card,Case Card ,Disease, kera,worm</t>
   </si>
 </sst>
 </file>
@@ -1895,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D50" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,7 +1929,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1955,35 +1955,35 @@
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>355</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>356</v>
       </c>
       <c r="E3" s="5"/>
       <c r="G3" s="35" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E4" s="7"/>
       <c r="G4" s="36"/>
@@ -1991,16 +1991,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E5" s="7"/>
       <c r="G5" s="36"/>
@@ -2008,16 +2008,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E6" s="7"/>
       <c r="G6" s="36"/>
@@ -2025,16 +2025,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E7" s="7"/>
       <c r="G7" s="36"/>
@@ -2042,16 +2042,16 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>342</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>343</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>350</v>
-      </c>
       <c r="D8" s="26" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E8" s="9"/>
       <c r="G8" s="36"/>
@@ -2111,7 +2111,7 @@
         <v>79</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G11" s="31"/>
       <c r="H11" s="14"/>
@@ -2184,7 +2184,7 @@
         <v>84</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>86</v>
@@ -2206,7 +2206,7 @@
         <v>100</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G16" s="31"/>
       <c r="H16" s="14"/>
@@ -2480,7 +2480,7 @@
         <v>164</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G30" s="33"/>
       <c r="H30" s="14"/>
@@ -2613,7 +2613,7 @@
         <v>176</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G37" s="33"/>
       <c r="H37" s="14"/>
@@ -2767,7 +2767,7 @@
         <v>188</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G45" s="33"/>
       <c r="H45" s="14"/>
@@ -2786,7 +2786,7 @@
         <v>189</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G46" s="33"/>
       <c r="H46" s="17" t="s">
@@ -2868,7 +2868,7 @@
         <v>272</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G50" s="33"/>
       <c r="H50" s="14"/>
@@ -2925,7 +2925,7 @@
         <v>299</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G53" s="33"/>
       <c r="H53" s="14"/>
@@ -2998,10 +2998,10 @@
         <v>294</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>306</v>
+        <v>367</v>
       </c>
       <c r="G57" s="33"/>
       <c r="H57" s="14"/>
@@ -3017,10 +3017,10 @@
         <v>295</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G58" s="33"/>
       <c r="H58" s="14"/>
@@ -3036,7 +3036,7 @@
         <v>296</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>305</v>
@@ -3058,7 +3058,7 @@
         <v>100</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G60" s="33"/>
       <c r="H60" s="14"/>
@@ -3071,13 +3071,13 @@
         <v>237</v>
       </c>
       <c r="C61" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="D61" s="6" t="s">
-        <v>316</v>
-      </c>
       <c r="E61" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G61" s="33"/>
       <c r="H61" s="14"/>
@@ -3090,13 +3090,13 @@
         <v>238</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G62" s="33"/>
       <c r="H62" s="14"/>
@@ -3112,10 +3112,10 @@
         <v>273</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G63" s="33"/>
       <c r="H63" s="14"/>
@@ -3131,10 +3131,10 @@
         <v>274</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G64" s="33"/>
       <c r="H64" s="14"/>
@@ -3150,10 +3150,10 @@
         <v>275</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G65" s="33"/>
       <c r="H65" s="14"/>
@@ -3169,10 +3169,10 @@
         <v>276</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G66" s="33"/>
       <c r="H66" s="14"/>
@@ -3188,10 +3188,10 @@
         <v>277</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G67" s="33"/>
       <c r="H67" s="14"/>
@@ -3204,13 +3204,13 @@
         <v>244</v>
       </c>
       <c r="C68" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="D68" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="E68" s="7" t="s">
         <v>331</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>332</v>
       </c>
       <c r="G68" s="33"/>
       <c r="H68" s="14"/>
@@ -3226,10 +3226,10 @@
         <v>278</v>
       </c>
       <c r="D69" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="E69" s="7" t="s">
         <v>334</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>335</v>
       </c>
       <c r="G69" s="33"/>
       <c r="H69" s="14"/>
@@ -3248,7 +3248,7 @@
         <v>189</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G70" s="33"/>
       <c r="H70" s="14"/>
@@ -3267,7 +3267,7 @@
         <v>190</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G71" s="33"/>
       <c r="H71" s="14"/>
@@ -3396,20 +3396,20 @@
     </row>
     <row r="80" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>360</v>
-      </c>
       <c r="D80" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E80" s="3"/>
       <c r="G80" s="29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H80" s="14"/>
     </row>

</xml_diff>

<commit_message>
Updated for verifications in Home and investigation and configuration 3 file
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2112F9-9A64-475F-B894-E4065A2BB875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE7F272-D263-4D6C-8181-942EF89E7D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="369">
   <si>
     <t>Skin Care, This is to analyse about the skin</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Corona</t>
   </si>
   <si>
-    <t>Corona, To analysis the impact of the virus</t>
-  </si>
-  <si>
     <t>Skin Care, SetName1</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>Skin Care, CompName1</t>
   </si>
   <si>
-    <t>Skin Care</t>
-  </si>
-  <si>
     <t>Test Case#</t>
   </si>
   <si>
@@ -1138,6 +1132,15 @@
   </si>
   <si>
     <t>DComparison2Card, Control Card,Case Card ,Disease, kera,worm</t>
+  </si>
+  <si>
+    <t>Skin Care, Corona, To analysis the impact of the virus</t>
+  </si>
+  <si>
+    <t>Skin Care 1</t>
+  </si>
+  <si>
+    <t>Skin Care, mugunth.raman@eaglegenomics.com</t>
   </si>
 </sst>
 </file>
@@ -1895,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="C69" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72:E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1914,76 +1917,76 @@
   <sheetData>
     <row r="1" spans="1:8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
       <c r="H1" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E3" s="5"/>
       <c r="G3" s="35" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>353</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>355</v>
       </c>
       <c r="E4" s="7"/>
       <c r="G4" s="36"/>
@@ -1991,16 +1994,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E5" s="7"/>
       <c r="G5" s="36"/>
@@ -2008,16 +2011,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E6" s="7"/>
       <c r="G6" s="36"/>
@@ -2025,16 +2028,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E7" s="7"/>
       <c r="G7" s="36"/>
@@ -2042,16 +2045,16 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E8" s="9"/>
       <c r="G8" s="36"/>
@@ -2059,1225 +2062,1225 @@
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="G9" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G10" s="31"/>
       <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G11" s="31"/>
       <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G12" s="31"/>
       <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G13" s="31"/>
       <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G14" s="31"/>
       <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="G15" s="31"/>
       <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G16" s="31"/>
       <c r="H16" s="14"/>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G17" s="31"/>
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G18" s="31"/>
       <c r="H18" s="17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G19" s="31"/>
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G20" s="31"/>
       <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G21" s="31"/>
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G22" s="31"/>
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G26" s="32"/>
       <c r="H26" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>158</v>
-      </c>
       <c r="G27" s="33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G28" s="33"/>
       <c r="H28" s="14"/>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G29" s="33"/>
       <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G30" s="33"/>
       <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D31" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>165</v>
       </c>
       <c r="G31" s="33"/>
       <c r="H31" s="14"/>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G32" s="33"/>
       <c r="H32" s="14"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G33" s="33"/>
       <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G34" s="33"/>
       <c r="H34" s="14"/>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G35" s="33"/>
       <c r="H35" s="14"/>
     </row>
     <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G36" s="33"/>
       <c r="H36" s="14"/>
     </row>
     <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G37" s="33"/>
       <c r="H37" s="14"/>
     </row>
     <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D38" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="G38" s="33"/>
       <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D39" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>180</v>
       </c>
       <c r="G39" s="33"/>
       <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G40" s="33"/>
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G41" s="33"/>
       <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G42" s="33"/>
       <c r="H42" s="14"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G43" s="33"/>
       <c r="H43" s="14"/>
     </row>
     <row r="44" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G44" s="33"/>
       <c r="H44" s="17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G45" s="33"/>
       <c r="H45" s="14"/>
     </row>
     <row r="46" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G46" s="33"/>
       <c r="H46" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G47" s="34"/>
       <c r="H47" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G48" s="38" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H48" s="14"/>
     </row>
     <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G49" s="33"/>
       <c r="H49" s="14"/>
     </row>
     <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G50" s="33"/>
       <c r="H50" s="14"/>
     </row>
     <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G51" s="33"/>
       <c r="H51" s="14"/>
     </row>
     <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G52" s="33"/>
       <c r="H52" s="14"/>
     </row>
     <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G53" s="33"/>
       <c r="H53" s="14"/>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G54" s="33"/>
       <c r="H54" s="14"/>
     </row>
     <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G55" s="33"/>
       <c r="H55" s="14"/>
     </row>
     <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G56" s="33"/>
       <c r="H56" s="14"/>
     </row>
     <row r="57" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G57" s="33"/>
       <c r="H57" s="14"/>
     </row>
     <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G58" s="33"/>
       <c r="H58" s="14"/>
     </row>
     <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G59" s="33"/>
       <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G60" s="33"/>
       <c r="H60" s="14"/>
     </row>
     <row r="61" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D61" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="E61" s="7" t="s">
         <v>315</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>317</v>
       </c>
       <c r="G61" s="33"/>
       <c r="H61" s="14"/>
     </row>
     <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C62" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="E62" s="7" t="s">
         <v>316</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>318</v>
       </c>
       <c r="G62" s="33"/>
       <c r="H62" s="14"/>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G63" s="33"/>
       <c r="H63" s="14"/>
     </row>
     <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G64" s="33"/>
       <c r="H64" s="14"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G65" s="33"/>
       <c r="H65" s="14"/>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G66" s="33"/>
       <c r="H66" s="14"/>
     </row>
     <row r="67" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G67" s="33"/>
       <c r="H67" s="14"/>
     </row>
     <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C68" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="E68" s="7" t="s">
         <v>329</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>331</v>
       </c>
       <c r="G68" s="33"/>
       <c r="H68" s="14"/>
     </row>
     <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G69" s="33"/>
       <c r="H69" s="14"/>
     </row>
     <row r="70" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G70" s="33"/>
       <c r="H70" s="14"/>
     </row>
     <row r="71" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G71" s="33"/>
       <c r="H71" s="14"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
@@ -3285,106 +3288,106 @@
         <v>0</v>
       </c>
       <c r="G72" s="35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H72" s="14"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
       <c r="E73" s="7" t="s">
-        <v>1</v>
+        <v>367</v>
       </c>
       <c r="G73" s="36"/>
       <c r="H73" s="14"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
       <c r="E74" s="7" t="s">
-        <v>2</v>
+        <v>366</v>
       </c>
       <c r="G74" s="36"/>
       <c r="H74" s="14"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G75" s="36"/>
       <c r="H75" s="14"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
       <c r="E76" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G76" s="36"/>
       <c r="H76" s="14"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G77" s="36"/>
       <c r="H77" s="14"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="7" t="s">
-        <v>6</v>
+        <v>368</v>
       </c>
       <c r="G78" s="36"/>
       <c r="H78" s="14"/>
     </row>
     <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
@@ -3396,20 +3399,20 @@
     </row>
     <row r="80" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="27" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E80" s="3"/>
       <c r="G80" s="29" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H80" s="14"/>
     </row>

</xml_diff>

<commit_message>
removed comments for all cases
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE7F272-D263-4D6C-8181-942EF89E7D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585BD158-7291-443C-AF65-6636562AF28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -1898,7 +1898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C69" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C68" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E72" sqref="E72:E79"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixes after Jan 4 2022 run
1) VerifyLogoVisibility_Test              --> changed profile name
2) Test data change for share
3) Share investigation                      --> included catch
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585BD158-7291-443C-AF65-6636562AF28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF5438F-E30C-48D6-8617-57AC143A10FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="371">
   <si>
     <t>Skin Care, This is to analyse about the skin</t>
   </si>
@@ -354,12 +354,6 @@
     <t>Delete Set1,Disease,kera</t>
   </si>
   <si>
-    <t>Share Set1,Disease,kera,mugunth.raman@eaglegenomics.com</t>
-  </si>
-  <si>
-    <t>GridSet,mugunth.raman@eaglegenomics.com</t>
-  </si>
-  <si>
     <t>SortSet, Disease, pero, EFO Name</t>
   </si>
   <si>
@@ -606,15 +600,9 @@
     <t>Delete Exp1,Disease,kera</t>
   </si>
   <si>
-    <t>Share Exp1,Disease,kera,mugunth.raman@eaglegenomics.com</t>
-  </si>
-  <si>
     <t>ExpAddFromSet</t>
   </si>
   <si>
-    <t>ExSearch 1,mugunth.raman@eaglegenomics.com</t>
-  </si>
-  <si>
     <t>Remove Item Exploration,RNA,asb,AL160411.1,AC060814.4,AL022100.1</t>
   </si>
   <si>
@@ -993,18 +981,12 @@
     <t>&lt;Comparison Name to be selected&gt;,&lt;Control Set Name&gt;,&lt;entity to be selected&gt;, &lt;search text for creating Comparison control&gt;</t>
   </si>
   <si>
-    <t>Share Com1, Control Set,Disease,kera,mugunth.raman@eaglegenomics.com</t>
-  </si>
-  <si>
     <t>&lt;Comparison Name to be selected&gt;,&lt;Control Set Name&gt;,&lt;entity to be selected&gt;, &lt;search text for creating Comparison control&gt;,&lt;mail Id To Share To&gt;</t>
   </si>
   <si>
     <t>search Comparison</t>
   </si>
   <si>
-    <t>ComAddfromFile 1,mugunth.raman@eaglegenomics.com</t>
-  </si>
-  <si>
     <t>&lt;ComparisonName to be deleted&gt;</t>
   </si>
   <si>
@@ -1140,7 +1122,31 @@
     <t>Skin Care 1</t>
   </si>
   <si>
-    <t>Skin Care, mugunth.raman@eaglegenomics.com</t>
+    <t>&lt;Profile Name&gt;</t>
+  </si>
+  <si>
+    <t>Mugunth Raman</t>
+  </si>
+  <si>
+    <t>Share Set1,Disease,kera,api-test-user@eagle-demos.eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>GridSet,api-test-user@eagle-demos.eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>Share Exp1,Disease,kera,api-test-user@eagle-demos.eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>ExSearch 1,api-test-user@eagle-demos.eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>Share Com1, Control Set,Disease,kera,api-test-user@eagle-demos.eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>ComAddfromFile 1,api-test-user@eagle-demos.eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>Skin Care, api-test-user@eagle-demos.eaglegenomics.com</t>
   </si>
 </sst>
 </file>
@@ -1433,7 +1439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1548,6 +1554,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1898,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C68" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72:E79"/>
+    <sheetView tabSelected="1" topLeftCell="C71" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1932,7 +1941,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1958,35 +1967,35 @@
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E3" s="5"/>
       <c r="G3" s="35" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E4" s="7"/>
       <c r="G4" s="36"/>
@@ -1994,33 +2003,35 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>353</v>
-      </c>
-      <c r="E5" s="7"/>
+        <v>344</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>362</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>363</v>
+      </c>
       <c r="G5" s="36"/>
       <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E6" s="7"/>
       <c r="G6" s="36"/>
@@ -2028,16 +2039,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E7" s="7"/>
       <c r="G7" s="36"/>
@@ -2045,16 +2056,16 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>347</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>353</v>
       </c>
       <c r="E8" s="9"/>
       <c r="G8" s="36"/>
@@ -2114,7 +2125,7 @@
         <v>77</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="G11" s="31"/>
       <c r="H11" s="14"/>
@@ -2187,7 +2198,7 @@
         <v>82</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>84</v>
@@ -2209,7 +2220,7 @@
         <v>98</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="G16" s="31"/>
       <c r="H16" s="14"/>
@@ -2251,7 +2262,7 @@
       </c>
       <c r="G18" s="31"/>
       <c r="H18" s="17" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2303,10 +2314,10 @@
         <v>89</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>106</v>
+        <v>364</v>
       </c>
       <c r="G21" s="31"/>
       <c r="H21" s="14"/>
@@ -2322,7 +2333,7 @@
         <v>90</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>68</v>
@@ -2341,10 +2352,10 @@
         <v>91</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>107</v>
+        <v>365</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="14"/>
@@ -2360,10 +2371,10 @@
         <v>92</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="14"/>
@@ -2379,14 +2390,14 @@
         <v>93</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2400,877 +2411,877 @@
         <v>94</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G26" s="32"/>
       <c r="H26" s="17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>156</v>
-      </c>
       <c r="G27" s="33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G28" s="33"/>
       <c r="H28" s="14"/>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G29" s="33"/>
       <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="G30" s="33"/>
       <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D31" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="G31" s="33"/>
       <c r="H31" s="14"/>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G32" s="33"/>
       <c r="H32" s="14"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G33" s="33"/>
       <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G34" s="33"/>
       <c r="H34" s="14"/>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G35" s="33"/>
       <c r="H35" s="14"/>
     </row>
     <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G36" s="33"/>
       <c r="H36" s="14"/>
     </row>
     <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="G37" s="33"/>
       <c r="H37" s="14"/>
     </row>
     <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D38" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>177</v>
       </c>
       <c r="G38" s="33"/>
       <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D39" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>178</v>
       </c>
       <c r="G39" s="33"/>
       <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G40" s="33"/>
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>190</v>
+        <v>366</v>
       </c>
       <c r="G41" s="33"/>
       <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G42" s="33"/>
       <c r="H42" s="14"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>192</v>
+        <v>367</v>
       </c>
       <c r="G43" s="33"/>
       <c r="H43" s="14"/>
     </row>
     <row r="44" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G44" s="33"/>
       <c r="H44" s="17" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="G45" s="33"/>
       <c r="H45" s="14"/>
     </row>
     <row r="46" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="G46" s="33"/>
       <c r="H46" s="17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G47" s="34"/>
       <c r="H47" s="17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="G48" s="38" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="H48" s="14"/>
     </row>
     <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G49" s="33"/>
       <c r="H49" s="14"/>
     </row>
     <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="G50" s="33"/>
       <c r="H50" s="14"/>
     </row>
     <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="G51" s="33"/>
       <c r="H51" s="14"/>
     </row>
     <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="G52" s="33"/>
       <c r="H52" s="14"/>
     </row>
     <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="G53" s="33"/>
       <c r="H53" s="14"/>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="G54" s="33"/>
       <c r="H54" s="14"/>
     </row>
     <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G55" s="33"/>
       <c r="H55" s="14"/>
     </row>
     <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="G56" s="33"/>
       <c r="H56" s="14"/>
     </row>
     <row r="57" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="G57" s="33"/>
       <c r="H57" s="14"/>
     </row>
     <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="G58" s="33"/>
       <c r="H58" s="14"/>
     </row>
     <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="G59" s="33"/>
       <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="G60" s="33"/>
       <c r="H60" s="14"/>
     </row>
     <row r="61" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="G61" s="33"/>
       <c r="H61" s="14"/>
     </row>
     <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="G62" s="33"/>
       <c r="H62" s="14"/>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="G63" s="33"/>
       <c r="H63" s="14"/>
     </row>
     <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>319</v>
+        <v>368</v>
       </c>
       <c r="G64" s="33"/>
       <c r="H64" s="14"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="G65" s="33"/>
       <c r="H65" s="14"/>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>322</v>
+        <v>369</v>
       </c>
       <c r="G66" s="33"/>
       <c r="H66" s="14"/>
     </row>
     <row r="67" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="G67" s="33"/>
       <c r="H67" s="14"/>
     </row>
     <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="G68" s="33"/>
       <c r="H68" s="14"/>
     </row>
     <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="G69" s="33"/>
       <c r="H69" s="14"/>
     </row>
     <row r="70" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="G70" s="33"/>
       <c r="H70" s="14"/>
     </row>
     <row r="71" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="G71" s="33"/>
       <c r="H71" s="14"/>
@@ -3288,7 +3299,7 @@
         <v>0</v>
       </c>
       <c r="G72" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H72" s="14"/>
     </row>
@@ -3302,7 +3313,7 @@
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
       <c r="E73" s="7" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="G73" s="36"/>
       <c r="H73" s="14"/>
@@ -3317,7 +3328,7 @@
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
       <c r="E74" s="7" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="G74" s="36"/>
       <c r="H74" s="14"/>
@@ -3377,7 +3388,7 @@
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="7" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="G78" s="36"/>
       <c r="H78" s="14"/>
@@ -3399,20 +3410,20 @@
     </row>
     <row r="80" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="27" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E80" s="3"/>
       <c r="G80" s="29" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="H80" s="14"/>
     </row>

</xml_diff>

<commit_message>
Updated for Comparison and Exploration error fixes
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF5438F-E30C-48D6-8617-57AC143A10FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFB8080-D179-40A9-9952-601314D17CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -1128,25 +1128,25 @@
     <t>Mugunth Raman</t>
   </si>
   <si>
-    <t>Share Set1,Disease,kera,api-test-user@eagle-demos.eaglegenomics.com</t>
-  </si>
-  <si>
-    <t>GridSet,api-test-user@eagle-demos.eaglegenomics.com</t>
-  </si>
-  <si>
-    <t>Share Exp1,Disease,kera,api-test-user@eagle-demos.eaglegenomics.com</t>
-  </si>
-  <si>
-    <t>ExSearch 1,api-test-user@eagle-demos.eaglegenomics.com</t>
-  </si>
-  <si>
-    <t>Share Com1, Control Set,Disease,kera,api-test-user@eagle-demos.eaglegenomics.com</t>
-  </si>
-  <si>
-    <t>ComAddfromFile 1,api-test-user@eagle-demos.eaglegenomics.com</t>
-  </si>
-  <si>
-    <t>Skin Care, api-test-user@eagle-demos.eaglegenomics.com</t>
+    <t>Share Set1,Disease,kera,ChandraSekhara.ReddyMoola@eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>GridSet,ChandraSekhara.ReddyMoola@eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>Share Exp1,Disease,kera,ChandraSekhara.ReddyMoola@eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>ExSearch 1,ChandraSekhara.ReddyMoola@eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>Share Com1, Control Set,Disease,kera,ChandraSekhara.ReddyMoola@eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>ComAddfromFile 1,ChandraSekhara.ReddyMoola@eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>Skin Care, ChandraSekhara.ReddyMoola@eaglegenomics.com</t>
   </si>
 </sst>
 </file>
@@ -1528,6 +1528,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1554,9 +1557,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1907,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C71" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,7 +1979,7 @@
         <v>347</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="36" t="s">
         <v>324</v>
       </c>
       <c r="H3" s="14"/>
@@ -1998,7 +1998,7 @@
         <v>347</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="G4" s="36"/>
+      <c r="G4" s="37"/>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2011,13 +2011,13 @@
       <c r="C5" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="30" t="s">
         <v>362</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="G5" s="36"/>
+      <c r="G5" s="37"/>
       <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2034,7 +2034,7 @@
         <v>347</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="G6" s="36"/>
+      <c r="G6" s="37"/>
       <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2051,7 +2051,7 @@
         <v>347</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="G7" s="36"/>
+      <c r="G7" s="37"/>
       <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2068,7 +2068,7 @@
         <v>347</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="G8" s="36"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
       <c r="E9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="31" t="s">
         <v>43</v>
       </c>
       <c r="H9" s="15"/>
@@ -2108,7 +2108,7 @@
       <c r="E10" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="31"/>
+      <c r="G10" s="32"/>
       <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2127,7 +2127,7 @@
       <c r="E11" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="G11" s="31"/>
+      <c r="G11" s="32"/>
       <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2146,7 +2146,7 @@
       <c r="E12" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G12" s="31"/>
+      <c r="G12" s="32"/>
       <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2165,7 +2165,7 @@
       <c r="E13" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="31"/>
+      <c r="G13" s="32"/>
       <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2184,7 +2184,7 @@
       <c r="E14" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="31"/>
+      <c r="G14" s="32"/>
       <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2203,7 +2203,7 @@
       <c r="E15" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="31"/>
+      <c r="G15" s="32"/>
       <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2222,7 +2222,7 @@
       <c r="E16" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="G16" s="31"/>
+      <c r="G16" s="32"/>
       <c r="H16" s="14"/>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
       <c r="E17" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G17" s="31"/>
+      <c r="G17" s="32"/>
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2260,7 +2260,7 @@
       <c r="E18" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="31"/>
+      <c r="G18" s="32"/>
       <c r="H18" s="17" t="s">
         <v>213</v>
       </c>
@@ -2281,7 +2281,7 @@
       <c r="E19" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G19" s="31"/>
+      <c r="G19" s="32"/>
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2300,7 +2300,7 @@
       <c r="E20" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G20" s="31"/>
+      <c r="G20" s="32"/>
       <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2319,7 +2319,7 @@
       <c r="E21" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="G21" s="31"/>
+      <c r="G21" s="32"/>
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2338,7 +2338,7 @@
       <c r="E22" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="31"/>
+      <c r="G22" s="32"/>
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2357,7 +2357,7 @@
       <c r="E23" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="G23" s="31"/>
+      <c r="G23" s="32"/>
       <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2376,7 +2376,7 @@
       <c r="E24" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G24" s="31"/>
+      <c r="G24" s="32"/>
       <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
       <c r="E25" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="G25" s="31"/>
+      <c r="G25" s="32"/>
       <c r="H25" s="17" t="s">
         <v>108</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="E26" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G26" s="32"/>
+      <c r="G26" s="33"/>
       <c r="H26" s="17" t="s">
         <v>108</v>
       </c>
@@ -2437,7 +2437,7 @@
       <c r="E27" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="G27" s="34" t="s">
         <v>151</v>
       </c>
       <c r="H27" s="14"/>
@@ -2458,7 +2458,7 @@
       <c r="E28" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="G28" s="33"/>
+      <c r="G28" s="34"/>
       <c r="H28" s="14"/>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2477,7 +2477,7 @@
       <c r="E29" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="G29" s="33"/>
+      <c r="G29" s="34"/>
       <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2496,7 +2496,7 @@
       <c r="E30" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="G30" s="33"/>
+      <c r="G30" s="34"/>
       <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2515,7 +2515,7 @@
       <c r="E31" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="G31" s="33"/>
+      <c r="G31" s="34"/>
       <c r="H31" s="14"/>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2534,7 +2534,7 @@
       <c r="E32" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="G32" s="33"/>
+      <c r="G32" s="34"/>
       <c r="H32" s="14"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2553,7 +2553,7 @@
       <c r="E33" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="G33" s="33"/>
+      <c r="G33" s="34"/>
       <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2572,7 +2572,7 @@
       <c r="E34" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="G34" s="33"/>
+      <c r="G34" s="34"/>
       <c r="H34" s="14"/>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2591,7 +2591,7 @@
       <c r="E35" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="G35" s="33"/>
+      <c r="G35" s="34"/>
       <c r="H35" s="14"/>
     </row>
     <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2610,7 +2610,7 @@
       <c r="E36" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G36" s="33"/>
+      <c r="G36" s="34"/>
       <c r="H36" s="14"/>
     </row>
     <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2629,7 +2629,7 @@
       <c r="E37" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="G37" s="33"/>
+      <c r="G37" s="34"/>
       <c r="H37" s="14"/>
     </row>
     <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2648,7 +2648,7 @@
       <c r="E38" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="G38" s="33"/>
+      <c r="G38" s="34"/>
       <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -2667,7 +2667,7 @@
       <c r="E39" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="G39" s="33"/>
+      <c r="G39" s="34"/>
       <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2686,7 +2686,7 @@
       <c r="E40" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="G40" s="33"/>
+      <c r="G40" s="34"/>
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2705,7 +2705,7 @@
       <c r="E41" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="G41" s="33"/>
+      <c r="G41" s="34"/>
       <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2724,7 +2724,7 @@
       <c r="E42" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="G42" s="33"/>
+      <c r="G42" s="34"/>
       <c r="H42" s="14"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2743,7 +2743,7 @@
       <c r="E43" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="G43" s="33"/>
+      <c r="G43" s="34"/>
       <c r="H43" s="14"/>
     </row>
     <row r="44" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2762,7 +2762,7 @@
       <c r="E44" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="G44" s="33"/>
+      <c r="G44" s="34"/>
       <c r="H44" s="17" t="s">
         <v>213</v>
       </c>
@@ -2783,7 +2783,7 @@
       <c r="E45" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="G45" s="33"/>
+      <c r="G45" s="34"/>
       <c r="H45" s="14"/>
     </row>
     <row r="46" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2802,7 +2802,7 @@
       <c r="E46" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="G46" s="33"/>
+      <c r="G46" s="34"/>
       <c r="H46" s="17" t="s">
         <v>108</v>
       </c>
@@ -2823,7 +2823,7 @@
       <c r="E47" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="G47" s="34"/>
+      <c r="G47" s="35"/>
       <c r="H47" s="17" t="s">
         <v>108</v>
       </c>
@@ -2844,7 +2844,7 @@
       <c r="E48" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="G48" s="38" t="s">
+      <c r="G48" s="39" t="s">
         <v>212</v>
       </c>
       <c r="H48" s="14"/>
@@ -2865,7 +2865,7 @@
       <c r="E49" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="G49" s="33"/>
+      <c r="G49" s="34"/>
       <c r="H49" s="14"/>
     </row>
     <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2884,7 +2884,7 @@
       <c r="E50" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="G50" s="33"/>
+      <c r="G50" s="34"/>
       <c r="H50" s="14"/>
     </row>
     <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2903,7 +2903,7 @@
       <c r="E51" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="G51" s="33"/>
+      <c r="G51" s="34"/>
       <c r="H51" s="14"/>
     </row>
     <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2922,7 +2922,7 @@
       <c r="E52" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="G52" s="33"/>
+      <c r="G52" s="34"/>
       <c r="H52" s="14"/>
     </row>
     <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2941,7 +2941,7 @@
       <c r="E53" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="G53" s="33"/>
+      <c r="G53" s="34"/>
       <c r="H53" s="14"/>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2960,7 +2960,7 @@
       <c r="E54" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="G54" s="33"/>
+      <c r="G54" s="34"/>
       <c r="H54" s="14"/>
     </row>
     <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2979,7 +2979,7 @@
       <c r="E55" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="G55" s="33"/>
+      <c r="G55" s="34"/>
       <c r="H55" s="14"/>
     </row>
     <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2998,7 +2998,7 @@
       <c r="E56" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="G56" s="33"/>
+      <c r="G56" s="34"/>
       <c r="H56" s="14"/>
     </row>
     <row r="57" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -3017,7 +3017,7 @@
       <c r="E57" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="G57" s="33"/>
+      <c r="G57" s="34"/>
       <c r="H57" s="14"/>
     </row>
     <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3036,7 +3036,7 @@
       <c r="E58" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="G58" s="33"/>
+      <c r="G58" s="34"/>
       <c r="H58" s="14"/>
     </row>
     <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3055,7 +3055,7 @@
       <c r="E59" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="G59" s="33"/>
+      <c r="G59" s="34"/>
       <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3074,7 +3074,7 @@
       <c r="E60" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="G60" s="33"/>
+      <c r="G60" s="34"/>
       <c r="H60" s="14"/>
     </row>
     <row r="61" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3093,7 +3093,7 @@
       <c r="E61" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="G61" s="33"/>
+      <c r="G61" s="34"/>
       <c r="H61" s="14"/>
     </row>
     <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3112,7 +3112,7 @@
       <c r="E62" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="G62" s="33"/>
+      <c r="G62" s="34"/>
       <c r="H62" s="14"/>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3131,7 +3131,7 @@
       <c r="E63" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="G63" s="33"/>
+      <c r="G63" s="34"/>
       <c r="H63" s="14"/>
     </row>
     <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3150,7 +3150,7 @@
       <c r="E64" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="G64" s="33"/>
+      <c r="G64" s="34"/>
       <c r="H64" s="14"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -3169,7 +3169,7 @@
       <c r="E65" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="G65" s="33"/>
+      <c r="G65" s="34"/>
       <c r="H65" s="14"/>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3188,7 +3188,7 @@
       <c r="E66" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="G66" s="33"/>
+      <c r="G66" s="34"/>
       <c r="H66" s="14"/>
     </row>
     <row r="67" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -3207,7 +3207,7 @@
       <c r="E67" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="G67" s="33"/>
+      <c r="G67" s="34"/>
       <c r="H67" s="14"/>
     </row>
     <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3226,7 +3226,7 @@
       <c r="E68" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="G68" s="33"/>
+      <c r="G68" s="34"/>
       <c r="H68" s="14"/>
     </row>
     <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3245,7 +3245,7 @@
       <c r="E69" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="G69" s="33"/>
+      <c r="G69" s="34"/>
       <c r="H69" s="14"/>
     </row>
     <row r="70" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3264,7 +3264,7 @@
       <c r="E70" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="G70" s="33"/>
+      <c r="G70" s="34"/>
       <c r="H70" s="14"/>
     </row>
     <row r="71" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3283,7 +3283,7 @@
       <c r="E71" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="G71" s="33"/>
+      <c r="G71" s="34"/>
       <c r="H71" s="14"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -3298,7 +3298,7 @@
       <c r="E72" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G72" s="35" t="s">
+      <c r="G72" s="36" t="s">
         <v>162</v>
       </c>
       <c r="H72" s="14"/>
@@ -3315,7 +3315,7 @@
       <c r="E73" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="G73" s="36"/>
+      <c r="G73" s="37"/>
       <c r="H73" s="14"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -3330,7 +3330,7 @@
       <c r="E74" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="G74" s="36"/>
+      <c r="G74" s="37"/>
       <c r="H74" s="14"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3345,7 +3345,7 @@
       <c r="E75" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G75" s="36"/>
+      <c r="G75" s="37"/>
       <c r="H75" s="14"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3360,7 +3360,7 @@
       <c r="E76" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G76" s="36"/>
+      <c r="G76" s="37"/>
       <c r="H76" s="14"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3375,7 +3375,7 @@
       <c r="E77" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G77" s="36"/>
+      <c r="G77" s="37"/>
       <c r="H77" s="14"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3390,7 +3390,7 @@
       <c r="E78" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="G78" s="36"/>
+      <c r="G78" s="37"/>
       <c r="H78" s="14"/>
     </row>
     <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3405,7 +3405,7 @@
       <c r="E79" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G79" s="37"/>
+      <c r="G79" s="38"/>
       <c r="H79" s="14"/>
     </row>
     <row r="80" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Gave comments for each methods and added partial method for Help and FAQ
HELP, MANUAL and FAQ need to be implemented to interact with new tab
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFB8080-D179-40A9-9952-601314D17CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAAF752-8461-44BC-AC4D-37B257147801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="377">
   <si>
     <t>Skin Care, This is to analyse about the skin</t>
   </si>
@@ -1147,13 +1147,31 @@
   </si>
   <si>
     <t>Skin Care, ChandraSekhara.ReddyMoola@eaglegenomics.com</t>
+  </si>
+  <si>
+    <t>VerifyContactHelpDesk_Test</t>
+  </si>
+  <si>
+    <t>VerifyUserManual_Test</t>
+  </si>
+  <si>
+    <t>VerifyFAQ_Test</t>
+  </si>
+  <si>
+    <t>VerifyContactHelpDesk</t>
+  </si>
+  <si>
+    <t>VerifyUserManual</t>
+  </si>
+  <si>
+    <t>VerifyFAQ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1198,6 +1216,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1439,7 +1464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1504,12 +1529,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1528,9 +1547,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1557,6 +1573,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1595,8 +1623,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}" name="Table2" displayName="Table2" ref="A1:E80" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E80" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}" name="Table2" displayName="Table2" ref="A1:E83" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E83" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{86135FFC-C988-4F48-82DC-A41C181BA09E}" name="Test Case#" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{C46EA655-3EFD-4B21-A644-8A7F51CB4F27}" name="FunctionName" dataDxfId="3"/>
@@ -1905,10 +1933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1975,11 +2003,11 @@
       <c r="C3" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="22" t="s">
         <v>347</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="33" t="s">
         <v>324</v>
       </c>
       <c r="H3" s="14"/>
@@ -1994,11 +2022,11 @@
       <c r="C4" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="23" t="s">
         <v>347</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="G4" s="37"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2011,13 +2039,13 @@
       <c r="C5" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="23" t="s">
         <v>362</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="G5" s="37"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2030,11 +2058,11 @@
       <c r="C6" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>347</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="G6" s="37"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2047,1393 +2075,1444 @@
       <c r="C7" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="23" t="s">
         <v>347</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="G7" s="37"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="20" t="s">
         <v>334</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="23" t="s">
         <v>347</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="G8" s="37"/>
+      <c r="E8" s="7"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="14"/>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="15"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>374</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>371</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>374</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>347</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="32"/>
+      <c r="A10" s="38" t="s">
+        <v>375</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>372</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>375</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>347</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="14"/>
     </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="G11" s="32"/>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="39" t="s">
+        <v>376</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>373</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>376</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>347</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="29"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="G14" s="29"/>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G12" s="32"/>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="G15" s="29"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="32"/>
-      <c r="H13" s="14"/>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G14" s="32"/>
-      <c r="H14" s="14"/>
-    </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" s="32"/>
-      <c r="H15" s="14"/>
-    </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="G16" s="32"/>
+      <c r="G16" s="29"/>
       <c r="H16" s="14"/>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="G17" s="32"/>
+        <v>83</v>
+      </c>
+      <c r="G17" s="29"/>
       <c r="H17" s="14"/>
     </row>
-    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>102</v>
+        <v>302</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G18" s="32"/>
-      <c r="H18" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="G18" s="29"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G19" s="32"/>
+        <v>353</v>
+      </c>
+      <c r="G19" s="29"/>
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>99</v>
       </c>
       <c r="E20" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="29"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="29"/>
+      <c r="H21" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" s="29"/>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G20" s="32"/>
-      <c r="H20" s="14"/>
-    </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="G21" s="32"/>
-      <c r="H21" s="14"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" s="32"/>
-      <c r="H22" s="14"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="G23" s="32"/>
+      <c r="G23" s="29"/>
       <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="G24" s="29"/>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" s="29"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G24" s="32"/>
-      <c r="H24" s="14"/>
-    </row>
-    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="G27" s="29"/>
+      <c r="H27" s="14"/>
+    </row>
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E28" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="G25" s="32"/>
-      <c r="H25" s="17" t="s">
+      <c r="G28" s="29"/>
+      <c r="H28" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+    <row r="29" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="17" t="s">
+      <c r="G29" s="30"/>
+      <c r="H29" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="G27" s="34" t="s">
+      <c r="G30" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="H27" s="14"/>
-    </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="G28" s="34"/>
-      <c r="H28" s="14"/>
-    </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="G29" s="34"/>
-      <c r="H29" s="14"/>
-    </row>
-    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="G30" s="34"/>
       <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="G31" s="34"/>
+        <v>158</v>
+      </c>
+      <c r="G31" s="31"/>
       <c r="H31" s="14"/>
     </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="G32" s="34"/>
+        <v>157</v>
+      </c>
+      <c r="G32" s="31"/>
       <c r="H32" s="14"/>
     </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="G33" s="34"/>
+        <v>354</v>
+      </c>
+      <c r="G33" s="31"/>
       <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G34" s="31"/>
+      <c r="H34" s="14"/>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="G35" s="31"/>
+      <c r="H35" s="14"/>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G36" s="31"/>
+      <c r="H36" s="14"/>
+    </row>
+    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E37" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="G34" s="34"/>
-      <c r="H34" s="14"/>
-    </row>
-    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G35" s="34"/>
-      <c r="H35" s="14"/>
-    </row>
-    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G36" s="34"/>
-      <c r="H36" s="14"/>
-    </row>
-    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="G37" s="34"/>
+      <c r="G37" s="31"/>
       <c r="H37" s="14"/>
     </row>
     <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="G38" s="34"/>
+        <v>166</v>
+      </c>
+      <c r="G38" s="31"/>
       <c r="H38" s="14"/>
     </row>
-    <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="G39" s="34"/>
+        <v>167</v>
+      </c>
+      <c r="G39" s="31"/>
       <c r="H39" s="14"/>
     </row>
-    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="G40" s="34"/>
+        <v>355</v>
+      </c>
+      <c r="G40" s="31"/>
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="G41" s="34"/>
+        <v>175</v>
+      </c>
+      <c r="G41" s="31"/>
       <c r="H41" s="14"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="G42" s="34"/>
+        <v>176</v>
+      </c>
+      <c r="G42" s="31"/>
       <c r="H42" s="14"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="G43" s="31"/>
+      <c r="H43" s="14"/>
+    </row>
+    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="G44" s="31"/>
+      <c r="H44" s="14"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="G45" s="31"/>
+      <c r="H45" s="14"/>
+    </row>
+    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B46" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D46" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E46" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="G43" s="34"/>
-      <c r="H43" s="14"/>
-    </row>
-    <row r="44" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="G46" s="31"/>
+      <c r="H46" s="14"/>
+    </row>
+    <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B47" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D47" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E47" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="G44" s="34"/>
-      <c r="H44" s="17" t="s">
+      <c r="G47" s="31"/>
+      <c r="H47" s="17" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+    <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B48" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C48" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D48" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E48" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="G45" s="34"/>
-      <c r="H45" s="14"/>
-    </row>
-    <row r="46" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="G48" s="31"/>
+      <c r="H48" s="14"/>
+    </row>
+    <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B49" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C49" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E49" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="G46" s="34"/>
-      <c r="H46" s="17" t="s">
+      <c r="G49" s="31"/>
+      <c r="H49" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="12" t="s">
+    <row r="50" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B50" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C50" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E50" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="G47" s="35"/>
-      <c r="H47" s="17" t="s">
+      <c r="G50" s="32"/>
+      <c r="H50" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B51" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C51" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D51" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E51" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="G48" s="39" t="s">
+      <c r="G51" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="H48" s="14"/>
-    </row>
-    <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="H51" s="14"/>
+    </row>
+    <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B52" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C52" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D52" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E52" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="G49" s="34"/>
-      <c r="H49" s="14"/>
-    </row>
-    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="G50" s="34"/>
-      <c r="H50" s="14"/>
-    </row>
-    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="G51" s="34"/>
-      <c r="H51" s="14"/>
-    </row>
-    <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="G52" s="34"/>
+      <c r="G52" s="31"/>
       <c r="H52" s="14"/>
     </row>
     <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>293</v>
+        <v>266</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="G53" s="34"/>
+        <v>356</v>
+      </c>
+      <c r="G53" s="31"/>
       <c r="H53" s="14"/>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="G54" s="34"/>
+        <v>283</v>
+      </c>
+      <c r="G54" s="31"/>
       <c r="H54" s="14"/>
     </row>
-    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="G55" s="34"/>
+        <v>284</v>
+      </c>
+      <c r="G55" s="31"/>
       <c r="H55" s="14"/>
     </row>
     <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="G56" s="31"/>
+      <c r="H56" s="14"/>
+    </row>
+    <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="G57" s="31"/>
+      <c r="H57" s="14"/>
+    </row>
+    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="G58" s="31"/>
+      <c r="H58" s="14"/>
+    </row>
+    <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B59" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D59" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E59" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="G56" s="34"/>
-      <c r="H56" s="14"/>
-    </row>
-    <row r="57" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="G59" s="31"/>
+      <c r="H59" s="14"/>
+    </row>
+    <row r="60" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B60" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C60" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D60" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="E60" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="G57" s="34"/>
-      <c r="H57" s="14"/>
-    </row>
-    <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="G58" s="34"/>
-      <c r="H58" s="14"/>
-    </row>
-    <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="G59" s="34"/>
-      <c r="H59" s="14"/>
-    </row>
-    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="G60" s="34"/>
+      <c r="G60" s="31"/>
       <c r="H60" s="14"/>
     </row>
     <row r="61" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="G61" s="34"/>
+        <v>304</v>
+      </c>
+      <c r="G61" s="31"/>
       <c r="H61" s="14"/>
     </row>
     <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="G62" s="34"/>
+        <v>299</v>
+      </c>
+      <c r="G62" s="31"/>
       <c r="H62" s="14"/>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="G63" s="31"/>
+      <c r="H63" s="14"/>
+    </row>
+    <row r="64" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="G64" s="31"/>
+      <c r="H64" s="14"/>
+    </row>
+    <row r="65" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G65" s="31"/>
+      <c r="H65" s="14"/>
+    </row>
+    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B66" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C66" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D66" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E66" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="G63" s="34"/>
-      <c r="H63" s="14"/>
-    </row>
-    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+      <c r="G66" s="31"/>
+      <c r="H66" s="14"/>
+    </row>
+    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B67" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C67" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D67" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E67" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="G64" s="34"/>
-      <c r="H64" s="14"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+      <c r="G67" s="31"/>
+      <c r="H67" s="14"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B68" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C68" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="D68" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="E68" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="G65" s="34"/>
-      <c r="H65" s="14"/>
-    </row>
-    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
+      <c r="G68" s="31"/>
+      <c r="H68" s="14"/>
+    </row>
+    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B69" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C69" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D69" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="E66" s="7" t="s">
+      <c r="E69" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="G66" s="34"/>
-      <c r="H66" s="14"/>
-    </row>
-    <row r="67" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+      <c r="G69" s="31"/>
+      <c r="H69" s="14"/>
+    </row>
+    <row r="70" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B70" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C70" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D70" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="E67" s="7" t="s">
+      <c r="E70" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="G67" s="34"/>
-      <c r="H67" s="14"/>
-    </row>
-    <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+      <c r="G70" s="31"/>
+      <c r="H70" s="14"/>
+    </row>
+    <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B71" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C71" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="D71" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E71" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="G68" s="34"/>
-      <c r="H68" s="14"/>
-    </row>
-    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
+      <c r="G71" s="31"/>
+      <c r="H71" s="14"/>
+    </row>
+    <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B72" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C72" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="D72" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E72" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="G69" s="34"/>
-      <c r="H69" s="14"/>
-    </row>
-    <row r="70" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
+      <c r="G72" s="31"/>
+      <c r="H72" s="14"/>
+    </row>
+    <row r="73" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B73" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C73" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="D73" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E73" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="G70" s="34"/>
-      <c r="H70" s="14"/>
-    </row>
-    <row r="71" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="6" t="s">
+      <c r="G73" s="31"/>
+      <c r="H73" s="14"/>
+    </row>
+    <row r="74" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B74" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C74" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="D74" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="E71" s="7" t="s">
+      <c r="E74" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="G71" s="34"/>
-      <c r="H71" s="14"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="s">
+      <c r="G74" s="31"/>
+      <c r="H74" s="14"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="5" t="s">
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G72" s="36" t="s">
+      <c r="G75" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="H72" s="14"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="G73" s="37"/>
-      <c r="H73" s="14"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="G74" s="37"/>
-      <c r="H74" s="14"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6"/>
-      <c r="E75" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G75" s="37"/>
       <c r="H75" s="14"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
       <c r="E76" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G76" s="37"/>
+        <v>361</v>
+      </c>
+      <c r="G76" s="34"/>
       <c r="H76" s="14"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G77" s="37"/>
+        <v>360</v>
+      </c>
+      <c r="G77" s="34"/>
       <c r="H77" s="14"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G78" s="34"/>
+      <c r="H78" s="14"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G79" s="34"/>
+      <c r="H79" s="14"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G80" s="34"/>
+      <c r="H80" s="14"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="G78" s="37"/>
-      <c r="H78" s="14"/>
-    </row>
-    <row r="79" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="12" t="s">
+      <c r="G81" s="34"/>
+      <c r="H81" s="14"/>
+    </row>
+    <row r="82" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B82" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="9" t="s">
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G79" s="38"/>
-      <c r="H79" s="14"/>
-    </row>
-    <row r="80" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="27" t="s">
+      <c r="G82" s="35"/>
+      <c r="H82" s="14"/>
+    </row>
+    <row r="83" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="25" t="s">
         <v>350</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D80" s="28" t="s">
+      <c r="D83" s="26" t="s">
         <v>347</v>
       </c>
-      <c r="E80" s="3"/>
-      <c r="G80" s="29" t="s">
+      <c r="E83" s="3"/>
+      <c r="G83" s="27" t="s">
         <v>349</v>
       </c>
-      <c r="H80" s="14"/>
+      <c r="H83" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="G9:G26"/>
-    <mergeCell ref="G27:G47"/>
-    <mergeCell ref="G72:G79"/>
-    <mergeCell ref="G48:G71"/>
-    <mergeCell ref="G3:G8"/>
+    <mergeCell ref="G12:G29"/>
+    <mergeCell ref="G30:G50"/>
+    <mergeCell ref="G75:G82"/>
+    <mergeCell ref="G51:G74"/>
+    <mergeCell ref="G3:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Made changes to wait time for each of wait for save changes, edit and entities
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAAF752-8461-44BC-AC4D-37B257147801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BCB70B-191A-4472-9A90-ADC285401631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -1547,6 +1547,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1573,18 +1585,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1936,7 +1936,7 @@
   <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E11"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2007,7 +2007,7 @@
         <v>347</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="37" t="s">
         <v>324</v>
       </c>
       <c r="H3" s="14"/>
@@ -2026,7 +2026,7 @@
         <v>347</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="G4" s="34"/>
+      <c r="G4" s="38"/>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2045,7 +2045,7 @@
       <c r="E5" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="G5" s="34"/>
+      <c r="G5" s="38"/>
       <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2062,7 +2062,7 @@
         <v>347</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="G6" s="34"/>
+      <c r="G6" s="38"/>
       <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2079,7 +2079,7 @@
         <v>347</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="G7" s="34"/>
+      <c r="G7" s="38"/>
       <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2096,58 +2096,58 @@
         <v>347</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="G8" s="34"/>
+      <c r="G8" s="38"/>
       <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="29" t="s">
         <v>374</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="28" t="s">
         <v>374</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>347</v>
       </c>
       <c r="E9" s="7"/>
-      <c r="G9" s="34"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="29" t="s">
         <v>375</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="28" t="s">
         <v>372</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="28" t="s">
         <v>375</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>347</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="G10" s="34"/>
+      <c r="G10" s="38"/>
       <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="30" t="s">
         <v>376</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="31" t="s">
         <v>373</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="31" t="s">
         <v>376</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>347</v>
       </c>
       <c r="E11" s="9"/>
-      <c r="G11" s="34"/>
+      <c r="G11" s="38"/>
       <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2166,7 +2166,7 @@
       <c r="E12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="32" t="s">
         <v>43</v>
       </c>
       <c r="H12" s="15"/>
@@ -2187,7 +2187,7 @@
       <c r="E13" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="29"/>
+      <c r="G13" s="33"/>
       <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2206,7 +2206,7 @@
       <c r="E14" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="G14" s="29"/>
+      <c r="G14" s="33"/>
       <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2225,7 +2225,7 @@
       <c r="E15" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="29"/>
+      <c r="G15" s="33"/>
       <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
       <c r="E16" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G16" s="29"/>
+      <c r="G16" s="33"/>
       <c r="H16" s="14"/>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2263,7 +2263,7 @@
       <c r="E17" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G17" s="29"/>
+      <c r="G17" s="33"/>
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2282,7 +2282,7 @@
       <c r="E18" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="G18" s="29"/>
+      <c r="G18" s="33"/>
       <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2301,7 +2301,7 @@
       <c r="E19" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="G19" s="29"/>
+      <c r="G19" s="33"/>
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2320,7 +2320,7 @@
       <c r="E20" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G20" s="29"/>
+      <c r="G20" s="33"/>
       <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2339,7 +2339,7 @@
       <c r="E21" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="G21" s="29"/>
+      <c r="G21" s="33"/>
       <c r="H21" s="17" t="s">
         <v>213</v>
       </c>
@@ -2360,7 +2360,7 @@
       <c r="E22" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G22" s="29"/>
+      <c r="G22" s="33"/>
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2379,7 +2379,7 @@
       <c r="E23" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="G23" s="29"/>
+      <c r="G23" s="33"/>
       <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2398,7 +2398,7 @@
       <c r="E24" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="G24" s="29"/>
+      <c r="G24" s="33"/>
       <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2417,7 +2417,7 @@
       <c r="E25" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G25" s="29"/>
+      <c r="G25" s="33"/>
       <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2436,7 +2436,7 @@
       <c r="E26" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="G26" s="29"/>
+      <c r="G26" s="33"/>
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2455,7 +2455,7 @@
       <c r="E27" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G27" s="29"/>
+      <c r="G27" s="33"/>
       <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2474,7 +2474,7 @@
       <c r="E28" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="G28" s="29"/>
+      <c r="G28" s="33"/>
       <c r="H28" s="17" t="s">
         <v>108</v>
       </c>
@@ -2495,7 +2495,7 @@
       <c r="E29" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G29" s="30"/>
+      <c r="G29" s="34"/>
       <c r="H29" s="17" t="s">
         <v>108</v>
       </c>
@@ -2516,7 +2516,7 @@
       <c r="E30" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="G30" s="31" t="s">
+      <c r="G30" s="35" t="s">
         <v>151</v>
       </c>
       <c r="H30" s="14"/>
@@ -2537,7 +2537,7 @@
       <c r="E31" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="G31" s="31"/>
+      <c r="G31" s="35"/>
       <c r="H31" s="14"/>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2556,7 +2556,7 @@
       <c r="E32" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="G32" s="31"/>
+      <c r="G32" s="35"/>
       <c r="H32" s="14"/>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2575,7 +2575,7 @@
       <c r="E33" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="G33" s="31"/>
+      <c r="G33" s="35"/>
       <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2594,7 +2594,7 @@
       <c r="E34" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="G34" s="31"/>
+      <c r="G34" s="35"/>
       <c r="H34" s="14"/>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2613,7 +2613,7 @@
       <c r="E35" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="G35" s="31"/>
+      <c r="G35" s="35"/>
       <c r="H35" s="14"/>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2632,7 +2632,7 @@
       <c r="E36" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="G36" s="31"/>
+      <c r="G36" s="35"/>
       <c r="H36" s="14"/>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2651,7 +2651,7 @@
       <c r="E37" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="G37" s="31"/>
+      <c r="G37" s="35"/>
       <c r="H37" s="14"/>
     </row>
     <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2670,7 +2670,7 @@
       <c r="E38" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="G38" s="31"/>
+      <c r="G38" s="35"/>
       <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2689,7 +2689,7 @@
       <c r="E39" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G39" s="31"/>
+      <c r="G39" s="35"/>
       <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2708,7 +2708,7 @@
       <c r="E40" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="G40" s="31"/>
+      <c r="G40" s="35"/>
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2727,7 +2727,7 @@
       <c r="E41" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="G41" s="31"/>
+      <c r="G41" s="35"/>
       <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -2746,7 +2746,7 @@
       <c r="E42" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="G42" s="31"/>
+      <c r="G42" s="35"/>
       <c r="H42" s="14"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2765,7 +2765,7 @@
       <c r="E43" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="G43" s="31"/>
+      <c r="G43" s="35"/>
       <c r="H43" s="14"/>
     </row>
     <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2784,7 +2784,7 @@
       <c r="E44" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="G44" s="31"/>
+      <c r="G44" s="35"/>
       <c r="H44" s="14"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2803,7 +2803,7 @@
       <c r="E45" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="G45" s="31"/>
+      <c r="G45" s="35"/>
       <c r="H45" s="14"/>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2822,7 +2822,7 @@
       <c r="E46" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="G46" s="31"/>
+      <c r="G46" s="35"/>
       <c r="H46" s="14"/>
     </row>
     <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2841,7 +2841,7 @@
       <c r="E47" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="G47" s="31"/>
+      <c r="G47" s="35"/>
       <c r="H47" s="17" t="s">
         <v>213</v>
       </c>
@@ -2862,7 +2862,7 @@
       <c r="E48" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="G48" s="31"/>
+      <c r="G48" s="35"/>
       <c r="H48" s="14"/>
     </row>
     <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2881,7 +2881,7 @@
       <c r="E49" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="G49" s="31"/>
+      <c r="G49" s="35"/>
       <c r="H49" s="17" t="s">
         <v>108</v>
       </c>
@@ -2902,7 +2902,7 @@
       <c r="E50" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="G50" s="32"/>
+      <c r="G50" s="36"/>
       <c r="H50" s="17" t="s">
         <v>108</v>
       </c>
@@ -2923,7 +2923,7 @@
       <c r="E51" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="G51" s="36" t="s">
+      <c r="G51" s="40" t="s">
         <v>212</v>
       </c>
       <c r="H51" s="14"/>
@@ -2944,7 +2944,7 @@
       <c r="E52" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="G52" s="31"/>
+      <c r="G52" s="35"/>
       <c r="H52" s="14"/>
     </row>
     <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2963,7 +2963,7 @@
       <c r="E53" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="G53" s="31"/>
+      <c r="G53" s="35"/>
       <c r="H53" s="14"/>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2982,7 +2982,7 @@
       <c r="E54" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="G54" s="31"/>
+      <c r="G54" s="35"/>
       <c r="H54" s="14"/>
     </row>
     <row r="55" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3001,7 +3001,7 @@
       <c r="E55" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="G55" s="31"/>
+      <c r="G55" s="35"/>
       <c r="H55" s="14"/>
     </row>
     <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3020,7 +3020,7 @@
       <c r="E56" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="G56" s="31"/>
+      <c r="G56" s="35"/>
       <c r="H56" s="14"/>
     </row>
     <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3039,7 +3039,7 @@
       <c r="E57" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="G57" s="31"/>
+      <c r="G57" s="35"/>
       <c r="H57" s="14"/>
     </row>
     <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3058,7 +3058,7 @@
       <c r="E58" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="G58" s="31"/>
+      <c r="G58" s="35"/>
       <c r="H58" s="14"/>
     </row>
     <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3077,7 +3077,7 @@
       <c r="E59" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="G59" s="31"/>
+      <c r="G59" s="35"/>
       <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -3096,7 +3096,7 @@
       <c r="E60" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="G60" s="31"/>
+      <c r="G60" s="35"/>
       <c r="H60" s="14"/>
     </row>
     <row r="61" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3115,7 +3115,7 @@
       <c r="E61" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="G61" s="31"/>
+      <c r="G61" s="35"/>
       <c r="H61" s="14"/>
     </row>
     <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3134,7 +3134,7 @@
       <c r="E62" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="G62" s="31"/>
+      <c r="G62" s="35"/>
       <c r="H62" s="14"/>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3153,7 +3153,7 @@
       <c r="E63" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="G63" s="31"/>
+      <c r="G63" s="35"/>
       <c r="H63" s="14"/>
     </row>
     <row r="64" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3172,7 +3172,7 @@
       <c r="E64" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="G64" s="31"/>
+      <c r="G64" s="35"/>
       <c r="H64" s="14"/>
     </row>
     <row r="65" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3191,7 +3191,7 @@
       <c r="E65" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="G65" s="31"/>
+      <c r="G65" s="35"/>
       <c r="H65" s="14"/>
     </row>
     <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3210,7 +3210,7 @@
       <c r="E66" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="G66" s="31"/>
+      <c r="G66" s="35"/>
       <c r="H66" s="14"/>
     </row>
     <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3229,7 +3229,7 @@
       <c r="E67" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="G67" s="31"/>
+      <c r="G67" s="35"/>
       <c r="H67" s="14"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -3248,7 +3248,7 @@
       <c r="E68" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="G68" s="31"/>
+      <c r="G68" s="35"/>
       <c r="H68" s="14"/>
     </row>
     <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3267,7 +3267,7 @@
       <c r="E69" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="G69" s="31"/>
+      <c r="G69" s="35"/>
       <c r="H69" s="14"/>
     </row>
     <row r="70" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -3286,7 +3286,7 @@
       <c r="E70" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="G70" s="31"/>
+      <c r="G70" s="35"/>
       <c r="H70" s="14"/>
     </row>
     <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3305,7 +3305,7 @@
       <c r="E71" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="G71" s="31"/>
+      <c r="G71" s="35"/>
       <c r="H71" s="14"/>
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3324,7 +3324,7 @@
       <c r="E72" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="G72" s="31"/>
+      <c r="G72" s="35"/>
       <c r="H72" s="14"/>
     </row>
     <row r="73" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3343,7 +3343,7 @@
       <c r="E73" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="G73" s="31"/>
+      <c r="G73" s="35"/>
       <c r="H73" s="14"/>
     </row>
     <row r="74" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3362,7 +3362,7 @@
       <c r="E74" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="G74" s="31"/>
+      <c r="G74" s="35"/>
       <c r="H74" s="14"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3377,7 +3377,7 @@
       <c r="E75" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G75" s="33" t="s">
+      <c r="G75" s="37" t="s">
         <v>162</v>
       </c>
       <c r="H75" s="14"/>
@@ -3394,7 +3394,7 @@
       <c r="E76" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="G76" s="34"/>
+      <c r="G76" s="38"/>
       <c r="H76" s="14"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3409,7 +3409,7 @@
       <c r="E77" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="G77" s="34"/>
+      <c r="G77" s="38"/>
       <c r="H77" s="14"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3424,7 +3424,7 @@
       <c r="E78" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G78" s="34"/>
+      <c r="G78" s="38"/>
       <c r="H78" s="14"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3439,7 +3439,7 @@
       <c r="E79" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G79" s="34"/>
+      <c r="G79" s="38"/>
       <c r="H79" s="14"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3454,7 +3454,7 @@
       <c r="E80" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G80" s="34"/>
+      <c r="G80" s="38"/>
       <c r="H80" s="14"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3469,7 +3469,7 @@
       <c r="E81" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="G81" s="34"/>
+      <c r="G81" s="38"/>
       <c r="H81" s="14"/>
     </row>
     <row r="82" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3484,7 +3484,7 @@
       <c r="E82" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G82" s="35"/>
+      <c r="G82" s="39"/>
       <c r="H82" s="14"/>
     </row>
     <row r="83" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated some cases for Analysis (and modification for fails in other URLs)
Analysis cases were added and some modification were made for fails in other URL
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE344B7C-59FC-4462-AFB7-AAC8842DEE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D971A9-688B-428F-9AB5-64C77DC8130E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="385">
   <si>
     <t>Skin Care, This is to analyse about the skin</t>
   </si>
@@ -1159,6 +1159,36 @@
   </si>
   <si>
     <t>Check Login for valid credentials (Username and password given in Config properties file)</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>CreateAnalysis_Test</t>
+  </si>
+  <si>
+    <t>CreateAnalysisMandatoryCheck_Test</t>
+  </si>
+  <si>
+    <t>CreateAnalysis</t>
+  </si>
+  <si>
+    <t>CreateAnalysisMandatoryCheck</t>
+  </si>
+  <si>
+    <t>Create an analysis</t>
+  </si>
+  <si>
+    <t>&lt;AnalysisName&gt;, &lt;AnalysisDescription&gt;, &lt;studyName&gt;</t>
+  </si>
+  <si>
+    <t>Create an analysis after doing all the mandatory field check</t>
+  </si>
+  <si>
+    <t>Analysis-1,Analysis Description,Galleon</t>
+  </si>
+  <si>
+    <t>Analysis-2, Test Description for Analysis Check,Galleon</t>
   </si>
 </sst>
 </file>
@@ -1238,27 +1268,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="15">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1293,43 +1308,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1458,12 +1436,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1472,86 +1468,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1559,13 +1525,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1574,11 +1540,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1617,8 +1583,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}" name="Table2" displayName="Table2" ref="A1:E83" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E83" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}" name="Table2" displayName="Table2" ref="A1:E89" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E89" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{86135FFC-C988-4F48-82DC-A41C181BA09E}" name="Test Case#" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{C46EA655-3EFD-4B21-A644-8A7F51CB4F27}" name="FunctionName" dataDxfId="3"/>
@@ -1927,10 +1893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,1544 +1928,1621 @@
       <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="20" t="s">
         <v>344</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="G2" s="16" t="s">
+      <c r="E2" s="3"/>
+      <c r="G2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="14"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="20" t="s">
         <v>344</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="G3" s="37" t="s">
+      <c r="E3" s="3"/>
+      <c r="G3" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="H3" s="14"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>327</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="14"/>
+      <c r="E4" s="5"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="21" t="s">
         <v>359</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="14"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>335</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="14"/>
+      <c r="E6" s="5"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>336</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="18" t="s">
         <v>330</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="14"/>
+      <c r="E7" s="5"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="19" t="s">
         <v>337</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="14"/>
+      <c r="E8" s="5"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="24" t="s">
         <v>371</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="23" t="s">
         <v>368</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="23" t="s">
         <v>371</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="14"/>
+      <c r="E9" s="5"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="24" t="s">
         <v>372</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="23" t="s">
         <v>372</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="14"/>
+      <c r="E10" s="5"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="25" t="s">
         <v>373</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="26" t="s">
         <v>370</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="26" t="s">
         <v>373</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>344</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="14"/>
+      <c r="E11" s="7"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="15"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="33"/>
-      <c r="H13" s="14"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="14"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="14"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="14"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="14"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="14"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="14"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="G20" s="33"/>
-      <c r="H20" s="14"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="33"/>
-      <c r="H21" s="17" t="s">
+      <c r="G21" s="28"/>
+      <c r="H21" s="15" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="14"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="33"/>
-      <c r="H23" s="14"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="G24" s="33"/>
-      <c r="H24" s="14"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="33"/>
-      <c r="H25" s="14"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="14"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="G27" s="33"/>
-      <c r="H27" s="14"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G28" s="33"/>
-      <c r="H28" s="17" t="s">
+      <c r="G28" s="28"/>
+      <c r="H28" s="15" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="G29" s="34"/>
-      <c r="H29" s="17" t="s">
+      <c r="G29" s="29"/>
+      <c r="H29" s="15" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="G30" s="35" t="s">
+      <c r="G30" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="H30" s="14"/>
+      <c r="H30" s="12"/>
     </row>
     <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="G31" s="35"/>
-      <c r="H31" s="14"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="G32" s="35"/>
-      <c r="H32" s="14"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="G33" s="35"/>
-      <c r="H33" s="14"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="12"/>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="G34" s="35"/>
-      <c r="H34" s="14"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G35" s="35"/>
-      <c r="H35" s="14"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="12"/>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="G36" s="35"/>
-      <c r="H36" s="14"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="G37" s="35"/>
-      <c r="H37" s="14"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="12"/>
     </row>
     <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="G38" s="35"/>
-      <c r="H38" s="14"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="G39" s="35"/>
-      <c r="H39" s="14"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="E40" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="G40" s="35"/>
-      <c r="H40" s="14"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="G41" s="35"/>
-      <c r="H41" s="14"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="12"/>
     </row>
     <row r="42" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="G42" s="35"/>
-      <c r="H42" s="14"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E43" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="G43" s="35"/>
-      <c r="H43" s="14"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="12"/>
     </row>
     <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="G44" s="35"/>
-      <c r="H44" s="14"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="12"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E45" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="G45" s="35"/>
-      <c r="H45" s="14"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="12"/>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E46" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="G46" s="35"/>
-      <c r="H46" s="14"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="12"/>
     </row>
     <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="G47" s="35"/>
-      <c r="H47" s="17" t="s">
+      <c r="G47" s="30"/>
+      <c r="H47" s="15" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="G48" s="35"/>
-      <c r="H48" s="14"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="12"/>
     </row>
     <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D49" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="G49" s="35"/>
-      <c r="H49" s="17" t="s">
+      <c r="G49" s="30"/>
+      <c r="H49" s="15" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="E50" s="9" t="s">
+      <c r="E50" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="G50" s="36"/>
-      <c r="H50" s="17" t="s">
+      <c r="G50" s="31"/>
+      <c r="H50" s="15" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D51" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E51" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="G51" s="40" t="s">
+      <c r="G51" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="H51" s="14"/>
+      <c r="H51" s="12"/>
     </row>
     <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D52" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="E52" s="7" t="s">
+      <c r="E52" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="G52" s="35"/>
-      <c r="H52" s="14"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="12"/>
     </row>
     <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D53" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E53" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="G53" s="35"/>
-      <c r="H53" s="14"/>
+      <c r="G53" s="30"/>
+      <c r="H53" s="12"/>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E54" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="G54" s="35"/>
-      <c r="H54" s="14"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="12"/>
     </row>
     <row r="55" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D55" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E55" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="G55" s="35"/>
-      <c r="H55" s="14"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="12"/>
     </row>
     <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D56" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E56" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="G56" s="35"/>
-      <c r="H56" s="14"/>
+      <c r="G56" s="30"/>
+      <c r="H56" s="12"/>
     </row>
     <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="E57" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="G57" s="35"/>
-      <c r="H57" s="14"/>
+      <c r="G57" s="30"/>
+      <c r="H57" s="12"/>
     </row>
     <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="E58" s="7" t="s">
+      <c r="E58" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="G58" s="35"/>
-      <c r="H58" s="14"/>
+      <c r="G58" s="30"/>
+      <c r="H58" s="12"/>
     </row>
     <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="E59" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="G59" s="35"/>
-      <c r="H59" s="14"/>
+      <c r="G59" s="30"/>
+      <c r="H59" s="12"/>
     </row>
     <row r="60" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="E60" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="G60" s="35"/>
-      <c r="H60" s="14"/>
+      <c r="G60" s="30"/>
+      <c r="H60" s="12"/>
     </row>
     <row r="61" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="E61" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="G61" s="35"/>
-      <c r="H61" s="14"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="12"/>
     </row>
     <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E62" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="G62" s="35"/>
-      <c r="H62" s="14"/>
+      <c r="G62" s="30"/>
+      <c r="H62" s="12"/>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D63" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E63" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="G63" s="35"/>
-      <c r="H63" s="14"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="12"/>
     </row>
     <row r="64" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D64" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E64" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G64" s="35"/>
-      <c r="H64" s="14"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="12"/>
     </row>
     <row r="65" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="D65" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="E65" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="G65" s="35"/>
-      <c r="H65" s="14"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="12"/>
     </row>
     <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="E66" s="7" t="s">
+      <c r="E66" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="G66" s="35"/>
-      <c r="H66" s="14"/>
+      <c r="G66" s="30"/>
+      <c r="H66" s="12"/>
     </row>
     <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D67" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="E67" s="7" t="s">
+      <c r="E67" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="G67" s="35"/>
-      <c r="H67" s="14"/>
+      <c r="G67" s="30"/>
+      <c r="H67" s="12"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="D68" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E68" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="G68" s="35"/>
-      <c r="H68" s="14"/>
+      <c r="G68" s="30"/>
+      <c r="H68" s="12"/>
     </row>
     <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="D69" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E69" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="G69" s="35"/>
-      <c r="H69" s="14"/>
+      <c r="G69" s="30"/>
+      <c r="H69" s="12"/>
     </row>
     <row r="70" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="D70" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E70" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="G70" s="35"/>
-      <c r="H70" s="14"/>
+      <c r="G70" s="30"/>
+      <c r="H70" s="12"/>
     </row>
     <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C71" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="D71" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="E71" s="7" t="s">
+      <c r="E71" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="G71" s="35"/>
-      <c r="H71" s="14"/>
+      <c r="G71" s="30"/>
+      <c r="H71" s="12"/>
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="D72" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="E72" s="7" t="s">
+      <c r="E72" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="G72" s="35"/>
-      <c r="H72" s="14"/>
+      <c r="G72" s="30"/>
+      <c r="H72" s="12"/>
     </row>
     <row r="73" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
+      <c r="A73" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C73" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="D73" s="6" t="s">
+      <c r="D73" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="E73" s="7" t="s">
+      <c r="E73" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="G73" s="35"/>
-      <c r="H73" s="14"/>
+      <c r="G73" s="30"/>
+      <c r="H73" s="12"/>
     </row>
     <row r="74" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B74" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C74" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="D74" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="E74" s="7" t="s">
+      <c r="E74" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="G74" s="35"/>
-      <c r="H74" s="14"/>
+      <c r="G74" s="30"/>
+      <c r="H74" s="12"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="10" t="s">
+      <c r="A75" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="5" t="s">
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G75" s="37" t="s">
+      <c r="G75" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="H75" s="14"/>
+      <c r="H75" s="12"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="B76" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="7" t="s">
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="G76" s="38"/>
-      <c r="H76" s="14"/>
+      <c r="G76" s="33"/>
+      <c r="H76" s="12"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
+      <c r="A77" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="7" t="s">
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="G77" s="38"/>
-      <c r="H77" s="14"/>
+      <c r="G77" s="33"/>
+      <c r="H77" s="12"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
+      <c r="A78" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="7" t="s">
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G78" s="38"/>
-      <c r="H78" s="14"/>
+      <c r="G78" s="33"/>
+      <c r="H78" s="12"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
+      <c r="A79" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="7" t="s">
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G79" s="38"/>
-      <c r="H79" s="14"/>
+      <c r="G79" s="33"/>
+      <c r="H79" s="12"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B80" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="7" t="s">
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G80" s="38"/>
-      <c r="H80" s="14"/>
+      <c r="G80" s="33"/>
+      <c r="H80" s="12"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="B81" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="7" t="s">
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="G81" s="38"/>
-      <c r="H81" s="14"/>
+      <c r="G81" s="33"/>
+      <c r="H81" s="12"/>
     </row>
     <row r="82" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="12" t="s">
+      <c r="A82" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B82" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="9" t="s">
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G82" s="39"/>
-      <c r="H82" s="14"/>
-    </row>
-    <row r="83" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="25" t="s">
+      <c r="G82" s="33"/>
+      <c r="H82" s="12"/>
+    </row>
+    <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="G83" s="32" t="s">
+        <v>375</v>
+      </c>
+      <c r="H83" s="12"/>
+    </row>
+    <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="G84" s="33"/>
+      <c r="H84" s="12"/>
+    </row>
+    <row r="85" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="9"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="5"/>
+      <c r="G85" s="33"/>
+      <c r="H85" s="12"/>
+    </row>
+    <row r="86" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="9"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="5"/>
+      <c r="G86" s="33"/>
+      <c r="H86" s="12"/>
+    </row>
+    <row r="87" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="9"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="5"/>
+      <c r="G87" s="33"/>
+      <c r="H87" s="12"/>
+    </row>
+    <row r="88" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="10"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="7"/>
+      <c r="G88" s="34"/>
+      <c r="H88" s="12"/>
+    </row>
+    <row r="89" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B89" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C89" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="D83" s="26" t="s">
+      <c r="D89" s="22" t="s">
         <v>344</v>
       </c>
-      <c r="E83" s="3"/>
-      <c r="G83" s="27" t="s">
+      <c r="E89" s="7"/>
+      <c r="G89" s="36" t="s">
         <v>346</v>
       </c>
-      <c r="H83" s="14"/>
+      <c r="H89" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="G83:G88"/>
     <mergeCell ref="G12:G29"/>
     <mergeCell ref="G30:G50"/>
     <mergeCell ref="G75:G82"/>

</xml_diff>

<commit_message>
Added analysis cases for Numerical and categorical feature check
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D971A9-688B-428F-9AB5-64C77DC8130E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF31308-2BC1-49BE-8226-A18FC097C42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="406">
   <si>
     <t>Skin Care, This is to analyse about the skin</t>
   </si>
@@ -1185,10 +1185,73 @@
     <t>Create an analysis after doing all the mandatory field check</t>
   </si>
   <si>
-    <t>Analysis-1,Analysis Description,Galleon</t>
-  </si>
-  <si>
-    <t>Analysis-2, Test Description for Analysis Check,Galleon</t>
+    <t>AnalysisNameAndDescEditInList_Test</t>
+  </si>
+  <si>
+    <t>AnalysisNameAndDescEditInList</t>
+  </si>
+  <si>
+    <t>Create an Analysis and Edit the name and description from the list view</t>
+  </si>
+  <si>
+    <t>Analysis-1,Analysis Description,Eagle Study A</t>
+  </si>
+  <si>
+    <t>Analysis-2, Test Description for Analysis Check,Eagle Study A</t>
+  </si>
+  <si>
+    <t>Analysis-3,Analysis Description,Eagle Study A,Name of [Analysis&gt;: is changed, Description of [Analysis&gt;: is changed</t>
+  </si>
+  <si>
+    <t>Analysis-4,Far far away behind the word mountains far from the countries Vokalia and Consonantia there live the blind texts. Separated they live in Bookmarksgrove right at the coast of the Semantics a large language ocean. A small river named Duden flows by their place and supplies it with the necessary regelialia. It is a paradisematic country in which roasted parts of sentences fly into your mouth. Even the all-powerful Pointing has no control about the blind texts it is an almost unorthographic life One day however a small line of blind text by the name of Lorem Ipsum decided to leave for the far,Eagle Study A,Name of ()@#$Analysis{}: is changed, Description small, Description of ()@#$Analysis{}: is changed</t>
+  </si>
+  <si>
+    <t>AnalysisNameAndDescEditInPage_Test</t>
+  </si>
+  <si>
+    <t>AnalysisNameAndDescEditInPage</t>
+  </si>
+  <si>
+    <t>Create an Analysis and Edit the name and description inside the analysis page view</t>
+  </si>
+  <si>
+    <t>&lt;AnalysisNameInital&gt;, &lt;AnalysisDescriptionInital&gt;, &lt;StudyName&gt;, &lt;AnalysisName&gt;, &lt;AnalysisDescription&gt;</t>
+  </si>
+  <si>
+    <t>CreateAndDeleteAnalysis_Test</t>
+  </si>
+  <si>
+    <t>CreateAndDeleteAnalysis</t>
+  </si>
+  <si>
+    <t>Create an Analysis and Delete the same</t>
+  </si>
+  <si>
+    <t>Analysis-5,Analysis Description,Eagle Study A</t>
+  </si>
+  <si>
+    <t>VerifyNumericalValueAnalysis_Test</t>
+  </si>
+  <si>
+    <t>VerifyCategoticalValueAnalysis_Test</t>
+  </si>
+  <si>
+    <t>VerifyNumericalValueAnalysis</t>
+  </si>
+  <si>
+    <t>VerifyCategoticalValueAnalysis</t>
+  </si>
+  <si>
+    <t>Create an Analysis and select a Numerical feature and verify the labels</t>
+  </si>
+  <si>
+    <t>Numerical Value Analysis, Numerical Value Analysis, Eagle Study A,Subject,body_mass_index</t>
+  </si>
+  <si>
+    <t>&lt;AnalysisName&gt;, &lt;AnalysisDescription&gt;, &lt;studyName&gt;, &lt;Entity Name&gt;, &lt;Feature Name&gt;</t>
+  </si>
+  <si>
+    <t>Categorical Value Analysis, Categorical Value Analysis,Eagle Study A,Subject,disease</t>
   </si>
 </sst>
 </file>
@@ -1268,7 +1331,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1432,11 +1495,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1516,6 +1616,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1531,20 +1643,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1583,8 +1695,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}" name="Table2" displayName="Table2" ref="A1:E89" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E89" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}" name="Table2" displayName="Table2" ref="A1:E90" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E90" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{86135FFC-C988-4F48-82DC-A41C181BA09E}" name="Test Case#" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{C46EA655-3EFD-4B21-A644-8A7F51CB4F27}" name="FunctionName" dataDxfId="3"/>
@@ -1893,10 +2005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,7 +2077,7 @@
         <v>344</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="28" t="s">
         <v>321</v>
       </c>
       <c r="H3" s="12"/>
@@ -1984,7 +2096,7 @@
         <v>344</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="G4" s="33"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2003,7 +2115,7 @@
       <c r="E5" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="G5" s="33"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2020,7 +2132,7 @@
         <v>344</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="G6" s="33"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2037,7 +2149,7 @@
         <v>344</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="G7" s="33"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2054,7 +2166,7 @@
         <v>344</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="G8" s="33"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2071,7 +2183,7 @@
         <v>344</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="G9" s="33"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2088,7 +2200,7 @@
         <v>344</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="G10" s="33"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2105,7 +2217,7 @@
         <v>344</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="G11" s="33"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2124,7 +2236,7 @@
       <c r="E12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="31" t="s">
         <v>41</v>
       </c>
       <c r="H12" s="13"/>
@@ -2145,7 +2257,7 @@
       <c r="E13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="28"/>
+      <c r="G13" s="32"/>
       <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2164,7 +2276,7 @@
       <c r="E14" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="G14" s="28"/>
+      <c r="G14" s="32"/>
       <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2183,7 +2295,7 @@
       <c r="E15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="28"/>
+      <c r="G15" s="32"/>
       <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2202,7 +2314,7 @@
       <c r="E16" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="28"/>
+      <c r="G16" s="32"/>
       <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2221,7 +2333,7 @@
       <c r="E17" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G17" s="28"/>
+      <c r="G17" s="32"/>
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2240,7 +2352,7 @@
       <c r="E18" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="28"/>
+      <c r="G18" s="32"/>
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2259,7 +2371,7 @@
       <c r="E19" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="G19" s="28"/>
+      <c r="G19" s="32"/>
       <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2278,7 +2390,7 @@
       <c r="E20" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="G20" s="28"/>
+      <c r="G20" s="32"/>
       <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2297,7 +2409,7 @@
       <c r="E21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="28"/>
+      <c r="G21" s="32"/>
       <c r="H21" s="15" t="s">
         <v>210</v>
       </c>
@@ -2318,7 +2430,7 @@
       <c r="E22" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="28"/>
+      <c r="G22" s="32"/>
       <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2337,7 +2449,7 @@
       <c r="E23" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="28"/>
+      <c r="G23" s="32"/>
       <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2356,7 +2468,7 @@
       <c r="E24" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="G24" s="28"/>
+      <c r="G24" s="32"/>
       <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2375,7 +2487,7 @@
       <c r="E25" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="28"/>
+      <c r="G25" s="32"/>
       <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2394,7 +2506,7 @@
       <c r="E26" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="G26" s="28"/>
+      <c r="G26" s="32"/>
       <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2413,7 +2525,7 @@
       <c r="E27" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="G27" s="28"/>
+      <c r="G27" s="32"/>
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2432,7 +2544,7 @@
       <c r="E28" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G28" s="28"/>
+      <c r="G28" s="32"/>
       <c r="H28" s="15" t="s">
         <v>105</v>
       </c>
@@ -2453,7 +2565,7 @@
       <c r="E29" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="G29" s="29"/>
+      <c r="G29" s="33"/>
       <c r="H29" s="15" t="s">
         <v>105</v>
       </c>
@@ -2474,7 +2586,7 @@
       <c r="E30" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="G30" s="30" t="s">
+      <c r="G30" s="34" t="s">
         <v>148</v>
       </c>
       <c r="H30" s="12"/>
@@ -2495,7 +2607,7 @@
       <c r="E31" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="G31" s="30"/>
+      <c r="G31" s="34"/>
       <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2514,7 +2626,7 @@
       <c r="E32" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="G32" s="30"/>
+      <c r="G32" s="34"/>
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2533,7 +2645,7 @@
       <c r="E33" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="G33" s="30"/>
+      <c r="G33" s="34"/>
       <c r="H33" s="12"/>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2552,7 +2664,7 @@
       <c r="E34" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="G34" s="30"/>
+      <c r="G34" s="34"/>
       <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2571,7 +2683,7 @@
       <c r="E35" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G35" s="30"/>
+      <c r="G35" s="34"/>
       <c r="H35" s="12"/>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2590,7 +2702,7 @@
       <c r="E36" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="G36" s="30"/>
+      <c r="G36" s="34"/>
       <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2609,7 +2721,7 @@
       <c r="E37" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="G37" s="30"/>
+      <c r="G37" s="34"/>
       <c r="H37" s="12"/>
     </row>
     <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2628,7 +2740,7 @@
       <c r="E38" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="G38" s="30"/>
+      <c r="G38" s="34"/>
       <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2647,7 +2759,7 @@
       <c r="E39" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="G39" s="30"/>
+      <c r="G39" s="34"/>
       <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2666,7 +2778,7 @@
       <c r="E40" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="G40" s="30"/>
+      <c r="G40" s="34"/>
       <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2685,7 +2797,7 @@
       <c r="E41" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="G41" s="30"/>
+      <c r="G41" s="34"/>
       <c r="H41" s="12"/>
     </row>
     <row r="42" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -2704,7 +2816,7 @@
       <c r="E42" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="G42" s="30"/>
+      <c r="G42" s="34"/>
       <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2723,7 +2835,7 @@
       <c r="E43" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="G43" s="30"/>
+      <c r="G43" s="34"/>
       <c r="H43" s="12"/>
     </row>
     <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2742,7 +2854,7 @@
       <c r="E44" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="G44" s="30"/>
+      <c r="G44" s="34"/>
       <c r="H44" s="12"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2761,7 +2873,7 @@
       <c r="E45" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="G45" s="30"/>
+      <c r="G45" s="34"/>
       <c r="H45" s="12"/>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2780,7 +2892,7 @@
       <c r="E46" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="G46" s="30"/>
+      <c r="G46" s="34"/>
       <c r="H46" s="12"/>
     </row>
     <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2799,7 +2911,7 @@
       <c r="E47" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="G47" s="30"/>
+      <c r="G47" s="34"/>
       <c r="H47" s="15" t="s">
         <v>210</v>
       </c>
@@ -2820,7 +2932,7 @@
       <c r="E48" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="G48" s="30"/>
+      <c r="G48" s="34"/>
       <c r="H48" s="12"/>
     </row>
     <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2839,7 +2951,7 @@
       <c r="E49" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="G49" s="30"/>
+      <c r="G49" s="34"/>
       <c r="H49" s="15" t="s">
         <v>105</v>
       </c>
@@ -2860,7 +2972,7 @@
       <c r="E50" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="G50" s="31"/>
+      <c r="G50" s="35"/>
       <c r="H50" s="15" t="s">
         <v>105</v>
       </c>
@@ -2881,7 +2993,7 @@
       <c r="E51" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="G51" s="35" t="s">
+      <c r="G51" s="36" t="s">
         <v>209</v>
       </c>
       <c r="H51" s="12"/>
@@ -2902,7 +3014,7 @@
       <c r="E52" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="G52" s="30"/>
+      <c r="G52" s="34"/>
       <c r="H52" s="12"/>
     </row>
     <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2921,7 +3033,7 @@
       <c r="E53" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="G53" s="30"/>
+      <c r="G53" s="34"/>
       <c r="H53" s="12"/>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2940,7 +3052,7 @@
       <c r="E54" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="G54" s="30"/>
+      <c r="G54" s="34"/>
       <c r="H54" s="12"/>
     </row>
     <row r="55" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2959,7 +3071,7 @@
       <c r="E55" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="G55" s="30"/>
+      <c r="G55" s="34"/>
       <c r="H55" s="12"/>
     </row>
     <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2978,7 +3090,7 @@
       <c r="E56" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="G56" s="30"/>
+      <c r="G56" s="34"/>
       <c r="H56" s="12"/>
     </row>
     <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2997,7 +3109,7 @@
       <c r="E57" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="G57" s="30"/>
+      <c r="G57" s="34"/>
       <c r="H57" s="12"/>
     </row>
     <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3016,7 +3128,7 @@
       <c r="E58" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="G58" s="30"/>
+      <c r="G58" s="34"/>
       <c r="H58" s="12"/>
     </row>
     <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3035,7 +3147,7 @@
       <c r="E59" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="G59" s="30"/>
+      <c r="G59" s="34"/>
       <c r="H59" s="12"/>
     </row>
     <row r="60" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -3054,7 +3166,7 @@
       <c r="E60" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="G60" s="30"/>
+      <c r="G60" s="34"/>
       <c r="H60" s="12"/>
     </row>
     <row r="61" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3073,7 +3185,7 @@
       <c r="E61" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="G61" s="30"/>
+      <c r="G61" s="34"/>
       <c r="H61" s="12"/>
     </row>
     <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3092,7 +3204,7 @@
       <c r="E62" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="G62" s="30"/>
+      <c r="G62" s="34"/>
       <c r="H62" s="12"/>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3111,7 +3223,7 @@
       <c r="E63" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="G63" s="30"/>
+      <c r="G63" s="34"/>
       <c r="H63" s="12"/>
     </row>
     <row r="64" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3130,7 +3242,7 @@
       <c r="E64" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G64" s="30"/>
+      <c r="G64" s="34"/>
       <c r="H64" s="12"/>
     </row>
     <row r="65" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3149,7 +3261,7 @@
       <c r="E65" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="G65" s="30"/>
+      <c r="G65" s="34"/>
       <c r="H65" s="12"/>
     </row>
     <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3168,7 +3280,7 @@
       <c r="E66" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="G66" s="30"/>
+      <c r="G66" s="34"/>
       <c r="H66" s="12"/>
     </row>
     <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3187,7 +3299,7 @@
       <c r="E67" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="G67" s="30"/>
+      <c r="G67" s="34"/>
       <c r="H67" s="12"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -3206,7 +3318,7 @@
       <c r="E68" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="G68" s="30"/>
+      <c r="G68" s="34"/>
       <c r="H68" s="12"/>
     </row>
     <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3225,7 +3337,7 @@
       <c r="E69" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="G69" s="30"/>
+      <c r="G69" s="34"/>
       <c r="H69" s="12"/>
     </row>
     <row r="70" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -3244,7 +3356,7 @@
       <c r="E70" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="G70" s="30"/>
+      <c r="G70" s="34"/>
       <c r="H70" s="12"/>
     </row>
     <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3263,7 +3375,7 @@
       <c r="E71" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="G71" s="30"/>
+      <c r="G71" s="34"/>
       <c r="H71" s="12"/>
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3282,7 +3394,7 @@
       <c r="E72" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="G72" s="30"/>
+      <c r="G72" s="34"/>
       <c r="H72" s="12"/>
     </row>
     <row r="73" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3301,7 +3413,7 @@
       <c r="E73" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="G73" s="30"/>
+      <c r="G73" s="34"/>
       <c r="H73" s="12"/>
     </row>
     <row r="74" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3320,7 +3432,7 @@
       <c r="E74" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="G74" s="30"/>
+      <c r="G74" s="34"/>
       <c r="H74" s="12"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3335,7 +3447,7 @@
       <c r="E75" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G75" s="32" t="s">
+      <c r="G75" s="28" t="s">
         <v>159</v>
       </c>
       <c r="H75" s="12"/>
@@ -3352,7 +3464,7 @@
       <c r="E76" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="G76" s="33"/>
+      <c r="G76" s="29"/>
       <c r="H76" s="12"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3367,7 +3479,7 @@
       <c r="E77" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="G77" s="33"/>
+      <c r="G77" s="29"/>
       <c r="H77" s="12"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3382,7 +3494,7 @@
       <c r="E78" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G78" s="33"/>
+      <c r="G78" s="29"/>
       <c r="H78" s="12"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3397,7 +3509,7 @@
       <c r="E79" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G79" s="33"/>
+      <c r="G79" s="29"/>
       <c r="H79" s="12"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3412,7 +3524,7 @@
       <c r="E80" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G80" s="33"/>
+      <c r="G80" s="29"/>
       <c r="H80" s="12"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3427,7 +3539,7 @@
       <c r="E81" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="G81" s="33"/>
+      <c r="G81" s="29"/>
       <c r="H81" s="12"/>
     </row>
     <row r="82" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3442,7 +3554,7 @@
       <c r="E82" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G82" s="33"/>
+      <c r="G82" s="29"/>
       <c r="H82" s="12"/>
     </row>
     <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3459,9 +3571,9 @@
         <v>381</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="G83" s="32" t="s">
+        <v>386</v>
+      </c>
+      <c r="G83" s="28" t="s">
         <v>375</v>
       </c>
       <c r="H83" s="12"/>
@@ -3480,74 +3592,133 @@
         <v>381</v>
       </c>
       <c r="E84" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="G84" s="29"/>
+      <c r="H84" s="12"/>
+    </row>
+    <row r="85" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="G84" s="33"/>
-      <c r="H84" s="12"/>
-    </row>
-    <row r="85" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="9"/>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="5"/>
-      <c r="G85" s="33"/>
+      <c r="B85" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="G85" s="29"/>
       <c r="H85" s="12"/>
     </row>
-    <row r="86" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="9"/>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="5"/>
-      <c r="G86" s="33"/>
+    <row r="86" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="G86" s="29"/>
       <c r="H86" s="12"/>
     </row>
-    <row r="87" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="9"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="5"/>
-      <c r="G87" s="33"/>
+    <row r="87" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="G87" s="29"/>
       <c r="H87" s="12"/>
     </row>
-    <row r="88" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="10"/>
-      <c r="B88" s="6"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="7"/>
-      <c r="G88" s="34"/>
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="G88" s="29"/>
       <c r="H88" s="12"/>
     </row>
-    <row r="89" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="10" t="s">
+    <row r="89" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="G89" s="30"/>
+      <c r="H89" s="12"/>
+    </row>
+    <row r="90" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="37" t="s">
         <v>347</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B90" s="38" t="s">
         <v>345</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C90" s="38" t="s">
         <v>348</v>
       </c>
-      <c r="D89" s="22" t="s">
+      <c r="D90" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="E89" s="7"/>
-      <c r="G89" s="36" t="s">
+      <c r="E90" s="40"/>
+      <c r="G90" s="27" t="s">
         <v>346</v>
       </c>
-      <c r="H89" s="12"/>
+      <c r="H90" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="G83:G88"/>
+    <mergeCell ref="G3:G11"/>
+    <mergeCell ref="G83:G89"/>
     <mergeCell ref="G12:G29"/>
     <mergeCell ref="G30:G50"/>
     <mergeCell ref="G75:G82"/>
     <mergeCell ref="G51:G74"/>
-    <mergeCell ref="G3:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Made fixes for test cases (module) skip and partially completed analysis hub
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MugunthRaman\git\EagleAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF31308-2BC1-49BE-8226-A18FC097C42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D34CB7-CAC6-40F7-905F-6685DBF25396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3883F32-F6B7-4344-89C2-CDCBDBE1FA77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="420">
   <si>
     <t>Skin Care, This is to analyse about the skin</t>
   </si>
@@ -1252,13 +1252,57 @@
   </si>
   <si>
     <t>Categorical Value Analysis, Categorical Value Analysis,Eagle Study A,Subject,disease</t>
+  </si>
+  <si>
+    <t>VerifyGraphCanvas</t>
+  </si>
+  <si>
+    <t>VerifyGraphCanvas_Test</t>
+  </si>
+  <si>
+    <t>Verify if the graph canvas is displayed and the assosciated entities are present</t>
+  </si>
+  <si>
+    <t>VerifyResizingOfGraph_Test</t>
+  </si>
+  <si>
+    <t>VerifyResizingOfGraphCanvas</t>
+  </si>
+  <si>
+    <t>Verify if the expand and different views of Graph canvas are working fine</t>
+  </si>
+  <si>
+    <t>Resizing Graph Canvas Analysis, "Resizing Graph Canvas Analysis", "Eagle Study A"</t>
+  </si>
+  <si>
+    <t>Graph Canvas Analysis, Graph Canvas Analysis,Eagle Study A,5,The Study, Trial, Organism, Subject, Measurement</t>
+  </si>
+  <si>
+    <t>SelectCategoricalAndNumericalFeatures_Test</t>
+  </si>
+  <si>
+    <t>SelectCategoricalAndNumericalFeatures</t>
+  </si>
+  <si>
+    <t>Select Categorical and numerical features from Graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;AnalysisName&gt;, &lt;AnalysisDescription&gt;, &lt;studyName&gt;, &lt;NoOfEntities&gt;, &lt;Entitiy name 1&gt;, &lt;Entitiy name 2&gt;, &lt;Entitiy name 3&gt;, ….. &lt;Entitiy name (NoOfEntities)&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;AnalysisName&gt;, &lt;AnalysisDescription&gt;, &lt;studyName&gt;, &lt;NoOfEntitiyAndFeaturePairs&gt;, &lt;Entitiy name 1&gt;, &lt;Feature  name 1&gt;, &lt;Entitiy name 2&gt;, &lt;Feature  name 2&gt; ….. &lt;Entitiy name (NoOfEntities)&gt;, &lt;Feature  name (NoOfEntities)&gt;
+</t>
+  </si>
+  <si>
+    <t>Feature Selection Analysis, Feature Selection Analysis,Eagle Study A,5,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1306,6 +1350,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1536,7 +1588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1619,6 +1671,39 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1645,18 +1730,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1695,8 +1768,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}" name="Table2" displayName="Table2" ref="A1:E90" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E90" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}" name="Table2" displayName="Table2" ref="A1:E97" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:E97" xr:uid="{B81FA363-8335-4CA5-BD79-BF677456D3C2}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{86135FFC-C988-4F48-82DC-A41C181BA09E}" name="Test Case#" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{C46EA655-3EFD-4B21-A644-8A7F51CB4F27}" name="FunctionName" dataDxfId="3"/>
@@ -2005,9 +2078,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6CDC57-9314-4DDE-912B-780BF34D9001}">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
@@ -2077,7 +2150,7 @@
         <v>344</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="39" t="s">
         <v>321</v>
       </c>
       <c r="H3" s="12"/>
@@ -2096,7 +2169,7 @@
         <v>344</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="G4" s="29"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2115,7 +2188,7 @@
       <c r="E5" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="G5" s="29"/>
+      <c r="G5" s="40"/>
       <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2132,7 +2205,7 @@
         <v>344</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="G6" s="29"/>
+      <c r="G6" s="40"/>
       <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2149,7 +2222,7 @@
         <v>344</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="G7" s="29"/>
+      <c r="G7" s="40"/>
       <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2166,7 +2239,7 @@
         <v>344</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="G8" s="29"/>
+      <c r="G8" s="40"/>
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2183,7 +2256,7 @@
         <v>344</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="G9" s="29"/>
+      <c r="G9" s="40"/>
       <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2200,7 +2273,7 @@
         <v>344</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="G10" s="29"/>
+      <c r="G10" s="40"/>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2217,7 +2290,7 @@
         <v>344</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="G11" s="29"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2236,7 +2309,7 @@
       <c r="E12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="42" t="s">
         <v>41</v>
       </c>
       <c r="H12" s="13"/>
@@ -2257,7 +2330,7 @@
       <c r="E13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="32"/>
+      <c r="G13" s="43"/>
       <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2276,7 +2349,7 @@
       <c r="E14" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="G14" s="32"/>
+      <c r="G14" s="43"/>
       <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2295,7 +2368,7 @@
       <c r="E15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="32"/>
+      <c r="G15" s="43"/>
       <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2314,7 +2387,7 @@
       <c r="E16" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="32"/>
+      <c r="G16" s="43"/>
       <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2333,7 +2406,7 @@
       <c r="E17" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G17" s="32"/>
+      <c r="G17" s="43"/>
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2352,7 +2425,7 @@
       <c r="E18" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="32"/>
+      <c r="G18" s="43"/>
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2371,7 +2444,7 @@
       <c r="E19" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="G19" s="32"/>
+      <c r="G19" s="43"/>
       <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2390,7 +2463,7 @@
       <c r="E20" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="G20" s="32"/>
+      <c r="G20" s="43"/>
       <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2409,7 +2482,7 @@
       <c r="E21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="32"/>
+      <c r="G21" s="43"/>
       <c r="H21" s="15" t="s">
         <v>210</v>
       </c>
@@ -2430,7 +2503,7 @@
       <c r="E22" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="32"/>
+      <c r="G22" s="43"/>
       <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2449,7 +2522,7 @@
       <c r="E23" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="32"/>
+      <c r="G23" s="43"/>
       <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2468,7 +2541,7 @@
       <c r="E24" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="G24" s="32"/>
+      <c r="G24" s="43"/>
       <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2487,7 +2560,7 @@
       <c r="E25" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="32"/>
+      <c r="G25" s="43"/>
       <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2506,7 +2579,7 @@
       <c r="E26" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="G26" s="32"/>
+      <c r="G26" s="43"/>
       <c r="H26" s="12"/>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2525,7 +2598,7 @@
       <c r="E27" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="G27" s="32"/>
+      <c r="G27" s="43"/>
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2544,7 +2617,7 @@
       <c r="E28" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G28" s="32"/>
+      <c r="G28" s="43"/>
       <c r="H28" s="15" t="s">
         <v>105</v>
       </c>
@@ -2565,7 +2638,7 @@
       <c r="E29" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="G29" s="33"/>
+      <c r="G29" s="44"/>
       <c r="H29" s="15" t="s">
         <v>105</v>
       </c>
@@ -2586,7 +2659,7 @@
       <c r="E30" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="G30" s="34" t="s">
+      <c r="G30" s="45" t="s">
         <v>148</v>
       </c>
       <c r="H30" s="12"/>
@@ -2607,7 +2680,7 @@
       <c r="E31" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="G31" s="34"/>
+      <c r="G31" s="45"/>
       <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2626,7 +2699,7 @@
       <c r="E32" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="G32" s="34"/>
+      <c r="G32" s="45"/>
       <c r="H32" s="12"/>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2645,7 +2718,7 @@
       <c r="E33" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="G33" s="34"/>
+      <c r="G33" s="45"/>
       <c r="H33" s="12"/>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2664,7 +2737,7 @@
       <c r="E34" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="G34" s="34"/>
+      <c r="G34" s="45"/>
       <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2683,7 +2756,7 @@
       <c r="E35" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G35" s="34"/>
+      <c r="G35" s="45"/>
       <c r="H35" s="12"/>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2702,7 +2775,7 @@
       <c r="E36" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="G36" s="34"/>
+      <c r="G36" s="45"/>
       <c r="H36" s="12"/>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2721,7 +2794,7 @@
       <c r="E37" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="G37" s="34"/>
+      <c r="G37" s="45"/>
       <c r="H37" s="12"/>
     </row>
     <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2740,7 +2813,7 @@
       <c r="E38" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="G38" s="34"/>
+      <c r="G38" s="45"/>
       <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2759,7 +2832,7 @@
       <c r="E39" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="G39" s="34"/>
+      <c r="G39" s="45"/>
       <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2778,7 +2851,7 @@
       <c r="E40" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="G40" s="34"/>
+      <c r="G40" s="45"/>
       <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2797,7 +2870,7 @@
       <c r="E41" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="G41" s="34"/>
+      <c r="G41" s="45"/>
       <c r="H41" s="12"/>
     </row>
     <row r="42" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -2816,7 +2889,7 @@
       <c r="E42" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="G42" s="34"/>
+      <c r="G42" s="45"/>
       <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2835,7 +2908,7 @@
       <c r="E43" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="G43" s="34"/>
+      <c r="G43" s="45"/>
       <c r="H43" s="12"/>
     </row>
     <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2854,7 +2927,7 @@
       <c r="E44" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="G44" s="34"/>
+      <c r="G44" s="45"/>
       <c r="H44" s="12"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2873,7 +2946,7 @@
       <c r="E45" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="G45" s="34"/>
+      <c r="G45" s="45"/>
       <c r="H45" s="12"/>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2892,7 +2965,7 @@
       <c r="E46" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="G46" s="34"/>
+      <c r="G46" s="45"/>
       <c r="H46" s="12"/>
     </row>
     <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2911,7 +2984,7 @@
       <c r="E47" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="G47" s="34"/>
+      <c r="G47" s="45"/>
       <c r="H47" s="15" t="s">
         <v>210</v>
       </c>
@@ -2932,7 +3005,7 @@
       <c r="E48" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="G48" s="34"/>
+      <c r="G48" s="45"/>
       <c r="H48" s="12"/>
     </row>
     <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -2951,7 +3024,7 @@
       <c r="E49" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="G49" s="34"/>
+      <c r="G49" s="45"/>
       <c r="H49" s="15" t="s">
         <v>105</v>
       </c>
@@ -2972,7 +3045,7 @@
       <c r="E50" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="G50" s="35"/>
+      <c r="G50" s="46"/>
       <c r="H50" s="15" t="s">
         <v>105</v>
       </c>
@@ -2993,7 +3066,7 @@
       <c r="E51" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="G51" s="36" t="s">
+      <c r="G51" s="47" t="s">
         <v>209</v>
       </c>
       <c r="H51" s="12"/>
@@ -3014,7 +3087,7 @@
       <c r="E52" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="G52" s="34"/>
+      <c r="G52" s="45"/>
       <c r="H52" s="12"/>
     </row>
     <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3033,7 +3106,7 @@
       <c r="E53" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="G53" s="34"/>
+      <c r="G53" s="45"/>
       <c r="H53" s="12"/>
     </row>
     <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3052,7 +3125,7 @@
       <c r="E54" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="G54" s="34"/>
+      <c r="G54" s="45"/>
       <c r="H54" s="12"/>
     </row>
     <row r="55" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3071,7 +3144,7 @@
       <c r="E55" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="G55" s="34"/>
+      <c r="G55" s="45"/>
       <c r="H55" s="12"/>
     </row>
     <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3090,7 +3163,7 @@
       <c r="E56" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="G56" s="34"/>
+      <c r="G56" s="45"/>
       <c r="H56" s="12"/>
     </row>
     <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3109,7 +3182,7 @@
       <c r="E57" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="G57" s="34"/>
+      <c r="G57" s="45"/>
       <c r="H57" s="12"/>
     </row>
     <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3128,7 +3201,7 @@
       <c r="E58" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="G58" s="34"/>
+      <c r="G58" s="45"/>
       <c r="H58" s="12"/>
     </row>
     <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3147,7 +3220,7 @@
       <c r="E59" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="G59" s="34"/>
+      <c r="G59" s="45"/>
       <c r="H59" s="12"/>
     </row>
     <row r="60" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -3166,7 +3239,7 @@
       <c r="E60" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="G60" s="34"/>
+      <c r="G60" s="45"/>
       <c r="H60" s="12"/>
     </row>
     <row r="61" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3185,7 +3258,7 @@
       <c r="E61" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="G61" s="34"/>
+      <c r="G61" s="45"/>
       <c r="H61" s="12"/>
     </row>
     <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3204,7 +3277,7 @@
       <c r="E62" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="G62" s="34"/>
+      <c r="G62" s="45"/>
       <c r="H62" s="12"/>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3223,7 +3296,7 @@
       <c r="E63" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="G63" s="34"/>
+      <c r="G63" s="45"/>
       <c r="H63" s="12"/>
     </row>
     <row r="64" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3242,7 +3315,7 @@
       <c r="E64" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G64" s="34"/>
+      <c r="G64" s="45"/>
       <c r="H64" s="12"/>
     </row>
     <row r="65" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3261,7 +3334,7 @@
       <c r="E65" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="G65" s="34"/>
+      <c r="G65" s="45"/>
       <c r="H65" s="12"/>
     </row>
     <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3280,7 +3353,7 @@
       <c r="E66" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="G66" s="34"/>
+      <c r="G66" s="45"/>
       <c r="H66" s="12"/>
     </row>
     <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3299,7 +3372,7 @@
       <c r="E67" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="G67" s="34"/>
+      <c r="G67" s="45"/>
       <c r="H67" s="12"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -3318,7 +3391,7 @@
       <c r="E68" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="G68" s="34"/>
+      <c r="G68" s="45"/>
       <c r="H68" s="12"/>
     </row>
     <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3337,7 +3410,7 @@
       <c r="E69" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="G69" s="34"/>
+      <c r="G69" s="45"/>
       <c r="H69" s="12"/>
     </row>
     <row r="70" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -3356,7 +3429,7 @@
       <c r="E70" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="G70" s="34"/>
+      <c r="G70" s="45"/>
       <c r="H70" s="12"/>
     </row>
     <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3375,7 +3448,7 @@
       <c r="E71" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="G71" s="34"/>
+      <c r="G71" s="45"/>
       <c r="H71" s="12"/>
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3394,7 +3467,7 @@
       <c r="E72" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="G72" s="34"/>
+      <c r="G72" s="45"/>
       <c r="H72" s="12"/>
     </row>
     <row r="73" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3413,7 +3486,7 @@
       <c r="E73" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="G73" s="34"/>
+      <c r="G73" s="45"/>
       <c r="H73" s="12"/>
     </row>
     <row r="74" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3432,7 +3505,7 @@
       <c r="E74" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="G74" s="34"/>
+      <c r="G74" s="45"/>
       <c r="H74" s="12"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3447,7 +3520,7 @@
       <c r="E75" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G75" s="28" t="s">
+      <c r="G75" s="39" t="s">
         <v>159</v>
       </c>
       <c r="H75" s="12"/>
@@ -3464,7 +3537,7 @@
       <c r="E76" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="G76" s="29"/>
+      <c r="G76" s="40"/>
       <c r="H76" s="12"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3479,7 +3552,7 @@
       <c r="E77" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="G77" s="29"/>
+      <c r="G77" s="40"/>
       <c r="H77" s="12"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3494,7 +3567,7 @@
       <c r="E78" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G78" s="29"/>
+      <c r="G78" s="40"/>
       <c r="H78" s="12"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3509,7 +3582,7 @@
       <c r="E79" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G79" s="29"/>
+      <c r="G79" s="40"/>
       <c r="H79" s="12"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3524,7 +3597,7 @@
       <c r="E80" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G80" s="29"/>
+      <c r="G80" s="40"/>
       <c r="H80" s="12"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3539,7 +3612,7 @@
       <c r="E81" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="G81" s="29"/>
+      <c r="G81" s="40"/>
       <c r="H81" s="12"/>
     </row>
     <row r="82" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3554,7 +3627,7 @@
       <c r="E82" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G82" s="29"/>
+      <c r="G82" s="40"/>
       <c r="H82" s="12"/>
     </row>
     <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3573,7 +3646,7 @@
       <c r="E83" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="G83" s="28" t="s">
+      <c r="G83" s="39" t="s">
         <v>375</v>
       </c>
       <c r="H83" s="12"/>
@@ -3594,7 +3667,7 @@
       <c r="E84" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="G84" s="29"/>
+      <c r="G84" s="40"/>
       <c r="H84" s="12"/>
     </row>
     <row r="85" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3613,7 +3686,7 @@
       <c r="E85" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="G85" s="29"/>
+      <c r="G85" s="40"/>
       <c r="H85" s="12"/>
     </row>
     <row r="86" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.25">
@@ -3632,7 +3705,7 @@
       <c r="E86" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="G86" s="29"/>
+      <c r="G86" s="40"/>
       <c r="H86" s="12"/>
     </row>
     <row r="87" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3651,70 +3724,163 @@
       <c r="E87" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="G87" s="29"/>
+      <c r="G87" s="40"/>
       <c r="H87" s="12"/>
     </row>
-    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="D88" s="37" t="s">
+        <v>417</v>
+      </c>
+      <c r="E88" s="38" t="s">
+        <v>413</v>
+      </c>
+      <c r="G88" s="40"/>
+      <c r="H88" s="12"/>
+    </row>
+    <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="G89" s="40"/>
+      <c r="H89" s="12"/>
+    </row>
+    <row r="90" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C90" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="D90" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="E90" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="G88" s="29"/>
-      <c r="H88" s="12"/>
-    </row>
-    <row r="89" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="9" t="s">
+      <c r="G90" s="40"/>
+      <c r="H90" s="12"/>
+    </row>
+    <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C91" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="D91" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="E89" s="5" t="s">
+      <c r="E91" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="G89" s="30"/>
-      <c r="H89" s="12"/>
-    </row>
-    <row r="90" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="37" t="s">
+      <c r="G91" s="40"/>
+      <c r="H91" s="12"/>
+    </row>
+    <row r="92" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="D92" s="37" t="s">
+        <v>418</v>
+      </c>
+      <c r="E92" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="G92" s="40"/>
+      <c r="H92" s="12"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="9"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="5"/>
+      <c r="G93" s="40"/>
+      <c r="H93" s="12"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="9"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="5"/>
+      <c r="G94" s="40"/>
+      <c r="H94" s="12"/>
+    </row>
+    <row r="95" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="32"/>
+      <c r="B95" s="33"/>
+      <c r="C95" s="33"/>
+      <c r="D95" s="33"/>
+      <c r="E95" s="34"/>
+      <c r="G95" s="40"/>
+      <c r="H95" s="36"/>
+    </row>
+    <row r="96" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="9"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="5"/>
+      <c r="G96" s="41"/>
+      <c r="H96" s="12"/>
+    </row>
+    <row r="97" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="28" t="s">
         <v>347</v>
       </c>
-      <c r="B90" s="38" t="s">
+      <c r="B97" s="29" t="s">
         <v>345</v>
       </c>
-      <c r="C90" s="38" t="s">
+      <c r="C97" s="29" t="s">
         <v>348</v>
       </c>
-      <c r="D90" s="39" t="s">
+      <c r="D97" s="30" t="s">
         <v>344</v>
       </c>
-      <c r="E90" s="40"/>
-      <c r="G90" s="27" t="s">
+      <c r="E97" s="31"/>
+      <c r="G97" s="27" t="s">
         <v>346</v>
       </c>
-      <c r="H90" s="12"/>
+      <c r="H97" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="G3:G11"/>
-    <mergeCell ref="G83:G89"/>
+    <mergeCell ref="G83:G96"/>
     <mergeCell ref="G12:G29"/>
     <mergeCell ref="G30:G50"/>
     <mergeCell ref="G75:G82"/>

</xml_diff>

<commit_message>
Made change for fail in add from file, catalog and set. Added wait time of 2 secs to check name in my selection
</commit_message>
<xml_diff>
--- a/Resources/Configuration.xlsx
+++ b/Resources/Configuration.xlsx
@@ -3892,4 +3892,248 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005EDAA1EB1D58B449A665C8960057699D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70f6f9e5c7980eb9729804970d16a34b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="db720d58-4227-411f-bcee-c8e33b64d7b1" xmlns:ns3="63945a94-eccf-4e51-b06e-13c7875d9720" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="10a4f86fcee4fdd6d37add7357595ef5" ns2:_="" ns3:_="">
+    <xsd:import namespace="db720d58-4227-411f-bcee-c8e33b64d7b1"/>
+    <xsd:import namespace="63945a94-eccf-4e51-b06e-13c7875d9720"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="db720d58-4227-411f-bcee-c8e33b64d7b1" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="16" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="18" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="19" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="63945a94-eccf-4e51-b06e-13c7875d9720" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2499457-889B-40E7-BC5A-1F4DCBC44130}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{554B202B-FC5C-4B46-B8A4-E00F0F430312}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18F220F9-C131-4C9F-AAAD-C16DC24658DC}"/>
 </file>
</xml_diff>